<commit_message>
Commented three equation code
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_7_6.xlsx
+++ b/results/tables/final_tables_7_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A3CBD7-2B1C-4F7D-ADB6-5C0FEC8C5AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5FDA08-E133-45C2-BA26-B7A131918966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13410" yWindow="-17970" windowWidth="26040" windowHeight="14110" tabRatio="656" firstSheet="5" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="9" activeTab="12" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -25,12 +25,10 @@
     <sheet name="theta_estimates" sheetId="2" r:id="rId10"/>
     <sheet name="OLS_thetas" sheetId="8" r:id="rId11"/>
     <sheet name="sigma_estimates" sheetId="3" r:id="rId12"/>
-    <sheet name="top_jobs_skill" sheetId="5" r:id="rId13"/>
-    <sheet name="index_composition" sheetId="14" r:id="rId14"/>
+    <sheet name="pi_estimates" sheetId="16" r:id="rId13"/>
+    <sheet name="top_jobs_skill" sheetId="5" r:id="rId14"/>
+    <sheet name="index_composition" sheetId="14" r:id="rId15"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId15"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'step-up'!$E$9:$F$32</definedName>
   </definedNames>
@@ -100,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="276">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -889,6 +887,69 @@
   </si>
   <si>
     <t>Bachelor+</t>
+  </si>
+  <si>
+    <t>importance of: skill or accuracy in using hands/fingers</t>
+  </si>
+  <si>
+    <t>importance of: physical strength</t>
+  </si>
+  <si>
+    <t>importance of: physical stamina</t>
+  </si>
+  <si>
+    <t>importance of: dealing with people</t>
+  </si>
+  <si>
+    <t>importance of: working with a team</t>
+  </si>
+  <si>
+    <t>importance of: listening carefully to colleagues</t>
+  </si>
+  <si>
+    <t>importance of: making speeches/ presentations</t>
+  </si>
+  <si>
+    <t>importance of: persuading or influencing others</t>
+  </si>
+  <si>
+    <t>importance of: teaching people (individuals or groups)</t>
+  </si>
+  <si>
+    <t>how often work involves short repetitive tasks</t>
+  </si>
+  <si>
+    <t>influence personally have on: quality standards work to</t>
+  </si>
+  <si>
+    <t>how much variety in job</t>
+  </si>
+  <si>
+    <t>Importance of planning own act, bigger=less routine</t>
+  </si>
+  <si>
+    <t>importance of: writing long documents</t>
+  </si>
+  <si>
+    <t>importance of: reading long documents</t>
+  </si>
+  <si>
+    <t>importance of: arithmetic (adding, subtracting, multiplying, divid</t>
+  </si>
+  <si>
+    <t>importance of: arithmetic involving fractions (decimals, percentag</t>
+  </si>
+  <si>
+    <t>importance of: advanced mathematics/ statistics (using calculator/</t>
+  </si>
+  <si>
+    <t>importance of: planning the activities of others</t>
+  </si>
+  <si>
+    <t>importance of: thinking of solutions to problems</t>
+  </si>
+  <si>
+    <t>importance of: analysing complex problems in depth</t>
   </si>
 </sst>
 </file>
@@ -1295,6 +1356,8 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1340,8 +1403,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1538,24 +1599,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="index"/>
-      <sheetName val="correlation_colors"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2020,7 +2063,7 @@
   </sheetPr>
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2031,20 +2074,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="90" t="s">
+      <c r="G2" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2194,19 +2237,19 @@
       <c r="E8" s="74">
         <v>8.8865355218595204E-2</v>
       </c>
-      <c r="G8" s="92">
+      <c r="G8" s="77">
         <v>4.0630067214601502E-2</v>
       </c>
-      <c r="H8" s="92">
+      <c r="H8" s="77">
         <v>8.3571611908693402E-2</v>
       </c>
-      <c r="I8" s="92">
+      <c r="I8" s="77">
         <v>9.7324360517554401E-2</v>
       </c>
-      <c r="J8" s="92">
+      <c r="J8" s="77">
         <v>9.1894583020425705E-2</v>
       </c>
-      <c r="K8" s="92"/>
+      <c r="K8" s="77"/>
     </row>
     <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19"/>
@@ -2226,34 +2269,34 @@
         <f t="shared" si="3"/>
         <v>-7.0983830304353304E-2</v>
       </c>
-      <c r="G9" s="92">
+      <c r="G9" s="77">
         <v>3.6007782107965597E-2</v>
       </c>
-      <c r="H9" s="92">
+      <c r="H9" s="77">
         <v>0.106732211233662</v>
       </c>
-      <c r="I9" s="92">
+      <c r="I9" s="77">
         <v>9.9568615714996894E-2</v>
       </c>
-      <c r="J9" s="92">
+      <c r="J9" s="77">
         <v>0.124123017797548</v>
       </c>
-      <c r="K9" s="92"/>
+      <c r="K9" s="77"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G10" s="92">
+      <c r="G10" s="77">
         <v>3.4757427098277102E-2</v>
       </c>
-      <c r="H10" s="92">
+      <c r="H10" s="77">
         <v>9.6253137771482297E-2</v>
       </c>
-      <c r="I10" s="92">
+      <c r="I10" s="77">
         <v>0.102214538826463</v>
       </c>
-      <c r="J10" s="92">
+      <c r="J10" s="77">
         <v>7.0983830304353304E-2</v>
       </c>
-      <c r="K10" s="92"/>
+      <c r="K10" s="77"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
@@ -2287,11 +2330,11 @@
       <c r="B13" s="54">
         <v>62</v>
       </c>
-      <c r="G13" s="90" t="s">
+      <c r="G13" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
     </row>
     <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="G14" s="8" t="s">
@@ -2305,13 +2348,13 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="91" t="s">
+      <c r="A15" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
       <c r="G15" s="18">
         <f t="shared" ref="G15:I17" si="4">+C18/$B18</f>
         <v>2.2692799840412765</v>
@@ -2455,11 +2498,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="90" t="s">
+      <c r="G24" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="90"/>
-      <c r="I24" s="90"/>
+      <c r="H24" s="92"/>
+      <c r="I24" s="92"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -2485,13 +2528,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="91"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
+      <c r="B26" s="93"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
       <c r="G26" s="18">
         <f t="shared" ref="G26:I28" si="5">+C29/$B29</f>
         <v>1.0840988998256753</v>
@@ -2668,20 +2711,20 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="91" t="s">
+      <c r="A37" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="91"/>
-      <c r="C37" s="91"/>
-      <c r="D37" s="91"/>
-      <c r="E37" s="91"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="93"/>
+      <c r="D37" s="93"/>
+      <c r="E37" s="93"/>
     </row>
     <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="90" t="s">
+      <c r="G38" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="90"/>
-      <c r="I38" s="90"/>
+      <c r="H38" s="92"/>
+      <c r="I38" s="92"/>
     </row>
     <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -2798,7 +2841,7 @@
         <f>+E44/$B44</f>
         <v>0.15281934113026216</v>
       </c>
-      <c r="K42" s="92"/>
+      <c r="K42" s="77"/>
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="75">
@@ -2820,7 +2863,7 @@
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
       <c r="I43" s="18"/>
-      <c r="K43" s="92"/>
+      <c r="K43" s="77"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -2838,7 +2881,7 @@
       <c r="E44" s="74">
         <v>4.5849482279728501E-2</v>
       </c>
-      <c r="K44" s="92"/>
+      <c r="K44" s="77"/>
     </row>
     <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="19"/>
@@ -2858,31 +2901,31 @@
         <f t="shared" si="8"/>
         <v>-7.5233432632621805E-2</v>
       </c>
-      <c r="G45" s="93">
+      <c r="G45" s="78">
         <v>3.27791808747964E-2</v>
       </c>
-      <c r="H45" s="93">
+      <c r="H45" s="78">
         <v>7.5396741976460305E-2</v>
       </c>
-      <c r="I45" s="93">
+      <c r="I45" s="78">
         <v>0.115293505002319</v>
       </c>
-      <c r="J45" s="92">
+      <c r="J45" s="77">
         <v>0.14196233908585501</v>
       </c>
-      <c r="K45" s="92"/>
+      <c r="K45" s="77"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G46" s="92">
+      <c r="G46" s="77">
         <v>3.5902339137002803E-2</v>
       </c>
-      <c r="H46" s="92">
+      <c r="H46" s="77">
         <v>8.7285450730600303E-2</v>
       </c>
-      <c r="I46" s="92">
+      <c r="I46" s="77">
         <v>8.3582228841739506E-2</v>
       </c>
-      <c r="J46" s="92">
+      <c r="J46" s="77">
         <v>9.8175524348070906E-2</v>
       </c>
     </row>
@@ -2893,16 +2936,16 @@
       <c r="B47" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="G47" s="92">
+      <c r="G47" s="77">
         <v>3.5398027084865398E-2</v>
       </c>
-      <c r="H47" s="92">
+      <c r="H47" s="77">
         <v>8.8625088080741696E-2</v>
       </c>
-      <c r="I47" s="92">
+      <c r="I47" s="77">
         <v>8.7677991056143698E-2</v>
       </c>
-      <c r="J47" s="92">
+      <c r="J47" s="77">
         <v>7.5233432632621805E-2</v>
       </c>
     </row>
@@ -2922,10 +2965,10 @@
       <c r="E48" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="G48" s="92"/>
-      <c r="H48" s="92"/>
-      <c r="I48" s="92"/>
-      <c r="J48" s="92"/>
+      <c r="G48" s="77"/>
+      <c r="H48" s="77"/>
+      <c r="I48" s="77"/>
+      <c r="J48" s="77"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
@@ -2939,20 +2982,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A51" s="91" t="s">
+      <c r="A51" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="91"/>
-      <c r="C51" s="91"/>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
+      <c r="B51" s="93"/>
+      <c r="C51" s="93"/>
+      <c r="D51" s="93"/>
+      <c r="E51" s="93"/>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="90" t="s">
+      <c r="G52" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="90"/>
-      <c r="I52" s="90"/>
+      <c r="H52" s="92"/>
+      <c r="I52" s="92"/>
     </row>
     <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -3276,7 +3319,7 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3295,20 +3338,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="90" t="s">
+      <c r="G4" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -3488,8 +3531,8 @@
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3705,8 +3748,8 @@
       <c r="E18" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
       <c r="L18" s="35"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3871,13 +3914,320 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4C7DBF-8E9C-4E7A-AD2C-6A1AFD2D3CE0}">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A2:F33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" customWidth="1"/>
+    <col min="6" max="6" width="6.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="35"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="40"/>
+      <c r="C5" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="C6" s="9">
+        <v>-1.357559</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="47">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="9">
+        <v>-0.38607930000000001</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="48">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>-0.26557120000000001</v>
+      </c>
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="9">
+        <v>-8.2062300000000005E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="28">
+        <v>0.22691549999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C10" s="9"/>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="28">
+        <v>1.390266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="9">
+        <v>7.4287500000000006E-2</v>
+      </c>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="9"/>
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="28">
+        <v>1.932839</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.23517479999999999</v>
+      </c>
+      <c r="E13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="28">
+        <v>8.7551120000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.57731120000000002</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="49">
+        <v>102.45529999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="35">
+        <v>0.95</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1.1694340000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="45">
+        <v>0.99</v>
+      </c>
+      <c r="C16" s="46">
+        <v>5.8520029999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="35"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="40"/>
+      <c r="C21" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="E22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="47"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="48"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="F24" s="28"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="28"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C26" s="9"/>
+      <c r="E26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="28"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="F27" s="28"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C28" s="9"/>
+      <c r="E28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="28"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="28"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="E30" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="49"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="35">
+        <v>0.95</v>
+      </c>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="45">
+        <v>0.99</v>
+      </c>
+      <c r="C32" s="46"/>
+    </row>
+    <row r="33" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1118EAC5-EE01-4F6F-831E-9781C531891C}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A2:D19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -3904,12 +4254,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4104,12 +4454,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F0097E-5ADA-4F9F-8E43-EFEAF7A70026}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C27"/>
+    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4145,9 +4495,8 @@
       <c r="B4" t="s">
         <v>224</v>
       </c>
-      <c r="C4" t="e">
-        <f>+VLOOKUP(B4,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C4" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -4157,9 +4506,8 @@
       <c r="B5" t="s">
         <v>242</v>
       </c>
-      <c r="C5" t="e">
-        <f>+VLOOKUP(B5,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C5" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -4169,9 +4517,8 @@
       <c r="B6" t="s">
         <v>225</v>
       </c>
-      <c r="C6" t="e">
-        <f>+VLOOKUP(B6,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C6" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -4186,9 +4533,8 @@
       <c r="B8" t="s">
         <v>226</v>
       </c>
-      <c r="C8" t="e">
-        <f>+VLOOKUP(B8,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C8" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -4198,9 +4544,8 @@
       <c r="B9" t="s">
         <v>227</v>
       </c>
-      <c r="C9" t="e">
-        <f>+VLOOKUP(B9,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C9" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -4210,9 +4555,8 @@
       <c r="B10" t="s">
         <v>228</v>
       </c>
-      <c r="C10" t="e">
-        <f>+VLOOKUP(B10,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C10" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -4222,9 +4566,8 @@
       <c r="B11" t="s">
         <v>230</v>
       </c>
-      <c r="C11" t="e">
-        <f>+VLOOKUP(B11,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C11" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -4234,9 +4577,8 @@
       <c r="B12" t="s">
         <v>231</v>
       </c>
-      <c r="C12" t="e">
-        <f>+VLOOKUP(B12,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C12" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -4246,9 +4588,8 @@
       <c r="B13" t="s">
         <v>232</v>
       </c>
-      <c r="C13" t="e">
-        <f>+VLOOKUP(B13,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C13" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -4263,9 +4604,8 @@
       <c r="B15" t="s">
         <v>233</v>
       </c>
-      <c r="C15" t="e">
-        <f>+VLOOKUP(B15,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C15" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -4275,9 +4615,8 @@
       <c r="B16" t="s">
         <v>234</v>
       </c>
-      <c r="C16" t="e">
-        <f>+VLOOKUP(B16,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C16" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -4287,9 +4626,8 @@
       <c r="B17" t="s">
         <v>229</v>
       </c>
-      <c r="C17" t="e">
-        <f>+VLOOKUP(B17,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C17" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -4299,9 +4637,8 @@
       <c r="B18" t="s">
         <v>243</v>
       </c>
-      <c r="C18" t="e">
-        <f>+VLOOKUP(B18,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C18" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -4316,9 +4653,8 @@
       <c r="B20" t="s">
         <v>235</v>
       </c>
-      <c r="C20" t="e">
-        <f>+VLOOKUP(B20,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C20" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -4328,9 +4664,8 @@
       <c r="B21" t="s">
         <v>236</v>
       </c>
-      <c r="C21" t="e">
-        <f>+VLOOKUP(B21,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C21" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -4340,9 +4675,8 @@
       <c r="B22" t="s">
         <v>237</v>
       </c>
-      <c r="C22" t="e">
-        <f>+VLOOKUP(B22,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C22" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -4352,9 +4686,8 @@
       <c r="B23" t="s">
         <v>238</v>
       </c>
-      <c r="C23" t="e">
-        <f>+VLOOKUP(B23,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C23" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -4364,9 +4697,8 @@
       <c r="B24" t="s">
         <v>239</v>
       </c>
-      <c r="C24" t="e">
-        <f>+VLOOKUP(B24,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C24" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -4376,9 +4708,8 @@
       <c r="B25" t="s">
         <v>244</v>
       </c>
-      <c r="C25" t="e">
-        <f>+VLOOKUP(B25,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C25" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -4388,9 +4719,8 @@
       <c r="B26" t="s">
         <v>240</v>
       </c>
-      <c r="C26" t="e">
-        <f>+VLOOKUP(B26,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C26" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4400,9 +4730,8 @@
       <c r="B27" s="41" t="s">
         <v>241</v>
       </c>
-      <c r="C27" s="41" t="e">
-        <f>+VLOOKUP(B27,[1]!Table1[#Data],2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="C27" s="41" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -4494,66 +4823,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="79" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="79" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="N1" s="77" t="s">
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="N1" s="79" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="T1" s="77" t="s">
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="T1" s="79" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="80" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="78" t="s">
+      <c r="H2" s="80" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="N2" s="78" t="s">
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="N2" s="80" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="T2" s="78" t="s">
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="T2" s="80" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
+      <c r="W2" s="81"/>
+      <c r="X2" s="81"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -5585,10 +5914,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="80"/>
+      <c r="C2" s="82"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -6123,13 +6452,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6243,12 +6572,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -6547,12 +6876,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="82" t="s">
+      <c r="A37" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="82"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="84"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -6886,13 +7215,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="85" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -7130,13 +7459,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="84" t="s">
+      <c r="A21" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -7164,13 +7493,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="83" t="s">
+      <c r="A25" s="85" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -7432,13 +7761,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="84" t="s">
+      <c r="A43" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="84"/>
-      <c r="C43" s="84"/>
-      <c r="D43" s="84"/>
-      <c r="E43" s="84"/>
+      <c r="B43" s="86"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -7806,36 +8135,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="85"/>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="85"/>
-      <c r="Y3" s="85"/>
-      <c r="Z3" s="85"/>
-      <c r="AA3" s="85"/>
-      <c r="AB3" s="85"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="87"/>
+      <c r="AB3" s="87"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -8319,35 +8648,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="89" t="s">
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="86" t="s">
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87" t="s">
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="87"/>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="87"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="89"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>

<commit_message>
Added identifiers for the results
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_7_6.xlsx
+++ b/results/tables/final_tables_7_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5FDA08-E133-45C2-BA26-B7A131918966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312C4945-B38C-42C5-A737-43EE3720B6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="9" activeTab="12" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-19310" yWindow="-21840" windowWidth="38620" windowHeight="21100" tabRatio="656" activeTab="11" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="278">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -950,6 +950,12 @@
   </si>
   <si>
     <t>importance of: analysing complex problems in depth</t>
+  </si>
+  <si>
+    <t>Welch index</t>
+  </si>
+  <si>
+    <t>Correlation index</t>
   </si>
 </sst>
 </file>
@@ -1335,12 +1341,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1402,6 +1406,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1938,119 +1948,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7471085D-BC16-46A9-AF3A-D1F9FAE30012}">
-  <dimension ref="A2:F9"/>
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="15.1796875" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="90" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>254</v>
       </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="18">
+        <v>0.99999998999999995</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B4" s="18">
-        <v>0.99999998999999995</v>
-      </c>
-      <c r="C4" s="18"/>
+        <v>0.78706158000000004</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1</v>
+      </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>252</v>
+        <v>93</v>
       </c>
       <c r="B5" s="18">
-        <v>0.78706158000000004</v>
+        <v>0.36120983000000001</v>
       </c>
       <c r="C5" s="18">
-        <v>1</v>
-      </c>
-      <c r="D5" s="18"/>
+        <v>0.47599598999999998</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.99999998999999995</v>
+      </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="18">
+        <v>-6.5339869999999994E-2</v>
+      </c>
+      <c r="C6" s="18">
+        <v>4.1870570000000003E-2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.37941629999999998</v>
+      </c>
+      <c r="E6" s="18">
+        <v>1</v>
+      </c>
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="71">
+        <v>-0.62474819000000004</v>
+      </c>
+      <c r="C7" s="71">
+        <v>-0.72046911000000002</v>
+      </c>
+      <c r="D7" s="71">
+        <v>-0.84169570999999999</v>
+      </c>
+      <c r="E7" s="71">
+        <v>-0.57978885999999996</v>
+      </c>
+      <c r="F7" s="71">
+        <v>0.99999998999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="90" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" s="90"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="18">
-        <v>0.36120983000000001</v>
-      </c>
-      <c r="C6" s="18">
-        <v>0.47599598999999998</v>
-      </c>
-      <c r="D6" s="18">
-        <v>0.99999998999999995</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="E10" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="B7" s="18">
-        <v>-6.5339869999999994E-2</v>
-      </c>
-      <c r="C7" s="18">
-        <v>4.1870570000000003E-2</v>
-      </c>
-      <c r="D7" s="18">
-        <v>0.37941629999999998</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="F10" s="10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="18">
         <v>1</v>
       </c>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="18">
+        <v>0.86419999999999997</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="18">
+        <v>0.65110000000000001</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0.80120000000000002</v>
+      </c>
+      <c r="D13" s="18">
+        <v>1</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="18">
+        <v>0.45619999999999999</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0.628</v>
+      </c>
+      <c r="D14" s="18">
+        <v>0.83679999999999999</v>
+      </c>
+      <c r="E14" s="18">
+        <v>1</v>
+      </c>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B8" s="73">
-        <v>-0.62474819000000004</v>
-      </c>
-      <c r="C8" s="73">
-        <v>-0.72046911000000002</v>
-      </c>
-      <c r="D8" s="73">
-        <v>-0.84169570999999999</v>
-      </c>
-      <c r="E8" s="73">
-        <v>-0.57978885999999996</v>
-      </c>
-      <c r="F8" s="73">
-        <v>0.99999998999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="B15" s="71">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="C15" s="71">
+        <v>0.17519999999999999</v>
+      </c>
+      <c r="D15" s="71">
+        <v>0.3337</v>
+      </c>
+      <c r="E15" s="71">
+        <v>0.39879999999999999</v>
+      </c>
+      <c r="F15" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A9:F9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2063,8 +2199,8 @@
   </sheetPr>
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2074,20 +2210,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="92" t="s">
+      <c r="G2" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2119,16 +2255,16 @@
       <c r="A4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="74">
+      <c r="B4" s="72">
         <v>0.25355954851870199</v>
       </c>
-      <c r="C4" s="74">
+      <c r="C4" s="72">
         <v>0.26387458982134598</v>
       </c>
-      <c r="D4" s="74">
+      <c r="D4" s="72">
         <v>0.85431293094579996</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="72">
         <v>0.26031007955338298</v>
       </c>
       <c r="G4" s="18">
@@ -2145,19 +2281,19 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="75">
+      <c r="B5" s="73">
         <f>-G8</f>
         <v>-4.0630067214601502E-2</v>
       </c>
-      <c r="C5" s="75">
+      <c r="C5" s="73">
         <f t="shared" ref="C5:E5" si="1">-H8</f>
         <v>-8.3571611908693402E-2</v>
       </c>
-      <c r="D5" s="75">
+      <c r="D5" s="73">
         <f t="shared" si="1"/>
         <v>-9.7324360517554401E-2</v>
       </c>
-      <c r="E5" s="75">
+      <c r="E5" s="73">
         <f t="shared" si="1"/>
         <v>-9.1894583020425705E-2</v>
       </c>
@@ -2178,16 +2314,16 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="74">
+      <c r="B6" s="72">
         <v>0.25355954851870199</v>
       </c>
-      <c r="C6" s="74">
+      <c r="C6" s="72">
         <v>0.48810321482980101</v>
       </c>
-      <c r="D6" s="74">
+      <c r="D6" s="72">
         <v>0.76663404311067596</v>
       </c>
-      <c r="E6" s="74">
+      <c r="E6" s="72">
         <v>3.4831078331759503E-2</v>
       </c>
       <c r="G6" s="18">
@@ -2204,19 +2340,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="75">
+      <c r="B7" s="73">
         <f>+-G9</f>
         <v>-3.6007782107965597E-2</v>
       </c>
-      <c r="C7" s="75">
+      <c r="C7" s="73">
         <f t="shared" ref="C7:E7" si="2">+-H9</f>
         <v>-0.106732211233662</v>
       </c>
-      <c r="D7" s="75">
+      <c r="D7" s="73">
         <f t="shared" si="2"/>
         <v>-9.9568615714996894E-2</v>
       </c>
-      <c r="E7" s="75">
+      <c r="E7" s="73">
         <f t="shared" si="2"/>
         <v>-0.124123017797548</v>
       </c>
@@ -2225,78 +2361,78 @@
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="74">
+      <c r="B8" s="72">
         <v>0.25355954851870199</v>
       </c>
-      <c r="C8" s="74">
+      <c r="C8" s="72">
         <v>1.01519994788864</v>
       </c>
-      <c r="D8" s="74">
+      <c r="D8" s="72">
         <v>0.141187788574658</v>
       </c>
-      <c r="E8" s="74">
+      <c r="E8" s="72">
         <v>8.8865355218595204E-2</v>
       </c>
-      <c r="G8" s="77">
+      <c r="G8" s="75">
         <v>4.0630067214601502E-2</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="75">
         <v>8.3571611908693402E-2</v>
       </c>
-      <c r="I8" s="77">
+      <c r="I8" s="75">
         <v>9.7324360517554401E-2</v>
       </c>
-      <c r="J8" s="77">
+      <c r="J8" s="75">
         <v>9.1894583020425705E-2</v>
       </c>
-      <c r="K8" s="77"/>
+      <c r="K8" s="75"/>
     </row>
     <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19"/>
-      <c r="B9" s="76">
+      <c r="B9" s="74">
         <f>-G10</f>
         <v>-3.4757427098277102E-2</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="74">
         <f t="shared" ref="C9:E9" si="3">-H10</f>
         <v>-9.6253137771482297E-2</v>
       </c>
-      <c r="D9" s="76">
+      <c r="D9" s="74">
         <f t="shared" si="3"/>
         <v>-0.102214538826463</v>
       </c>
-      <c r="E9" s="76">
+      <c r="E9" s="74">
         <f t="shared" si="3"/>
         <v>-7.0983830304353304E-2</v>
       </c>
-      <c r="G9" s="77">
+      <c r="G9" s="75">
         <v>3.6007782107965597E-2</v>
       </c>
-      <c r="H9" s="77">
+      <c r="H9" s="75">
         <v>0.106732211233662</v>
       </c>
-      <c r="I9" s="77">
+      <c r="I9" s="75">
         <v>9.9568615714996894E-2</v>
       </c>
-      <c r="J9" s="77">
+      <c r="J9" s="75">
         <v>0.124123017797548</v>
       </c>
-      <c r="K9" s="77"/>
+      <c r="K9" s="75"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G10" s="77">
+      <c r="G10" s="75">
         <v>3.4757427098277102E-2</v>
       </c>
-      <c r="H10" s="77">
+      <c r="H10" s="75">
         <v>9.6253137771482297E-2</v>
       </c>
-      <c r="I10" s="77">
+      <c r="I10" s="75">
         <v>0.102214538826463</v>
       </c>
-      <c r="J10" s="77">
+      <c r="J10" s="75">
         <v>7.0983830304353304E-2</v>
       </c>
-      <c r="K10" s="77"/>
+      <c r="K10" s="75"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
@@ -2306,7 +2442,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
@@ -2323,20 +2459,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B13" s="54">
         <v>62</v>
       </c>
-      <c r="G13" s="92" t="s">
+      <c r="G13" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-    </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G14" s="8" t="s">
         <v>4</v>
       </c>
@@ -2348,13 +2484,13 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="93" t="s">
+      <c r="A15" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
       <c r="G15" s="18">
         <f t="shared" ref="G15:I17" si="4">+C18/$B18</f>
         <v>2.2692799840412765</v>
@@ -2368,7 +2504,7 @@
         <v>8.0096069126124061E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G16" s="18">
         <f t="shared" si="4"/>
         <v>2.4104194790539126</v>
@@ -2498,11 +2634,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="92" t="s">
+      <c r="G24" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -2528,13 +2664,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="93" t="s">
+      <c r="A26" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="93"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="93"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
       <c r="G26" s="18">
         <f t="shared" ref="G26:I28" si="5">+C29/$B29</f>
         <v>1.0840988998256753</v>
@@ -2560,7 +2696,7 @@
         <v>3.5119315719301103E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G27" s="18">
         <f t="shared" si="5"/>
         <v>2.2651573917720484</v>
@@ -2667,7 +2803,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>140</v>
       </c>
@@ -2675,7 +2811,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>19</v>
       </c>
@@ -2692,12 +2828,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B35" s="1">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2710,21 +2846,21 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="93" t="s">
+    <row r="37" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="93"/>
-      <c r="C37" s="93"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="93"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="91"/>
+      <c r="E37" s="91"/>
     </row>
     <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="92" t="s">
+      <c r="G38" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="92"/>
-      <c r="I38" s="92"/>
+      <c r="H38" s="90"/>
+      <c r="I38" s="90"/>
     </row>
     <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -2757,16 +2893,16 @@
       <c r="A40" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="74">
+      <c r="B40" s="72">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C40" s="74">
+      <c r="C40" s="72">
         <v>0.38983157888076198</v>
       </c>
-      <c r="D40" s="74">
+      <c r="D40" s="72">
         <v>0.77387006959986604</v>
       </c>
-      <c r="E40" s="74">
+      <c r="E40" s="72">
         <v>0.132595645940602</v>
       </c>
       <c r="G40" s="18">
@@ -2783,19 +2919,19 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B41" s="75">
+      <c r="B41" s="73">
         <f>-G45</f>
         <v>-3.27791808747964E-2</v>
       </c>
-      <c r="C41" s="75">
+      <c r="C41" s="73">
         <f t="shared" ref="C41:E41" si="6">-H45</f>
         <v>-7.5396741976460305E-2</v>
       </c>
-      <c r="D41" s="75">
+      <c r="D41" s="73">
         <f t="shared" si="6"/>
         <v>-0.115293505002319</v>
       </c>
-      <c r="E41" s="75">
+      <c r="E41" s="73">
         <f t="shared" si="6"/>
         <v>-0.14196233908585501</v>
       </c>
@@ -2817,16 +2953,16 @@
       <c r="A42" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="74">
+      <c r="B42" s="72">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C42" s="74">
+      <c r="C42" s="72">
         <v>0.536012038389163</v>
       </c>
-      <c r="D42" s="74">
+      <c r="D42" s="72">
         <v>0.65158108175637797</v>
       </c>
-      <c r="E42" s="74">
+      <c r="E42" s="72">
         <v>6.9889421558501405E-2</v>
       </c>
       <c r="G42" s="18">
@@ -2841,91 +2977,91 @@
         <f>+E44/$B44</f>
         <v>0.15281934113026216</v>
       </c>
-      <c r="K42" s="77"/>
+      <c r="K42" s="75"/>
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="75">
+      <c r="B43" s="73">
         <f>-G46</f>
         <v>-3.5902339137002803E-2</v>
       </c>
-      <c r="C43" s="75">
+      <c r="C43" s="73">
         <f t="shared" ref="C43:E43" si="7">-H46</f>
         <v>-8.7285450730600303E-2</v>
       </c>
-      <c r="D43" s="75">
+      <c r="D43" s="73">
         <f t="shared" si="7"/>
         <v>-8.3582228841739506E-2</v>
       </c>
-      <c r="E43" s="75">
+      <c r="E43" s="73">
         <f t="shared" si="7"/>
         <v>-9.8175524348070906E-2</v>
       </c>
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
       <c r="I43" s="18"/>
-      <c r="K43" s="77"/>
+      <c r="K43" s="75"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="74">
+      <c r="B44" s="72">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C44" s="74">
+      <c r="C44" s="72">
         <v>0.62828630817505104</v>
       </c>
-      <c r="D44" s="74">
+      <c r="D44" s="72">
         <v>0.55193979369233104</v>
       </c>
-      <c r="E44" s="74">
+      <c r="E44" s="72">
         <v>4.5849482279728501E-2</v>
       </c>
-      <c r="K44" s="77"/>
+      <c r="K44" s="75"/>
     </row>
     <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="19"/>
-      <c r="B45" s="76">
+      <c r="B45" s="74">
         <f>-G47</f>
         <v>-3.5398027084865398E-2</v>
       </c>
-      <c r="C45" s="76">
+      <c r="C45" s="74">
         <f t="shared" ref="C45:E45" si="8">-H47</f>
         <v>-8.8625088080741696E-2</v>
       </c>
-      <c r="D45" s="76">
+      <c r="D45" s="74">
         <f t="shared" si="8"/>
         <v>-8.7677991056143698E-2</v>
       </c>
-      <c r="E45" s="76">
+      <c r="E45" s="74">
         <f t="shared" si="8"/>
         <v>-7.5233432632621805E-2</v>
       </c>
-      <c r="G45" s="78">
+      <c r="G45" s="76">
         <v>3.27791808747964E-2</v>
       </c>
-      <c r="H45" s="78">
+      <c r="H45" s="76">
         <v>7.5396741976460305E-2</v>
       </c>
-      <c r="I45" s="78">
+      <c r="I45" s="76">
         <v>0.115293505002319</v>
       </c>
-      <c r="J45" s="77">
+      <c r="J45" s="75">
         <v>0.14196233908585501</v>
       </c>
-      <c r="K45" s="77"/>
+      <c r="K45" s="75"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G46" s="77">
+      <c r="G46" s="75">
         <v>3.5902339137002803E-2</v>
       </c>
-      <c r="H46" s="77">
+      <c r="H46" s="75">
         <v>8.7285450730600303E-2</v>
       </c>
-      <c r="I46" s="77">
+      <c r="I46" s="75">
         <v>8.3582228841739506E-2</v>
       </c>
-      <c r="J46" s="77">
+      <c r="J46" s="75">
         <v>9.8175524348070906E-2</v>
       </c>
     </row>
@@ -2936,16 +3072,16 @@
       <c r="B47" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="G47" s="77">
+      <c r="G47" s="75">
         <v>3.5398027084865398E-2</v>
       </c>
-      <c r="H47" s="77">
+      <c r="H47" s="75">
         <v>8.8625088080741696E-2</v>
       </c>
-      <c r="I47" s="77">
+      <c r="I47" s="75">
         <v>8.7677991056143698E-2</v>
       </c>
-      <c r="J47" s="77">
+      <c r="J47" s="75">
         <v>7.5233432632621805E-2</v>
       </c>
     </row>
@@ -2965,10 +3101,10 @@
       <c r="E48" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="G48" s="77"/>
-      <c r="H48" s="77"/>
-      <c r="I48" s="77"/>
-      <c r="J48" s="77"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
+      <c r="I48" s="75"/>
+      <c r="J48" s="75"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
@@ -2982,20 +3118,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A51" s="93" t="s">
+      <c r="A51" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="93"/>
-      <c r="C51" s="93"/>
-      <c r="D51" s="93"/>
-      <c r="E51" s="93"/>
+      <c r="B51" s="91"/>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="91"/>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="92" t="s">
+      <c r="G52" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="92"/>
-      <c r="I52" s="92"/>
+      <c r="H52" s="90"/>
+      <c r="I52" s="90"/>
     </row>
     <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -3319,7 +3455,7 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3338,20 +3474,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="92" t="s">
+      <c r="G4" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -3531,8 +3667,8 @@
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3728,7 +3864,7 @@
         <v>140</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L17" s="35"/>
     </row>
@@ -3748,8 +3884,8 @@
       <c r="E18" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80"/>
       <c r="L18" s="35"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3918,10 +4054,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A2:F33"/>
+  <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4089,8 +4225,8 @@
         <v>5.8520029999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>140</v>
       </c>
@@ -4098,7 +4234,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -4115,106 +4251,148 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="35"/>
     </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="40"/>
       <c r="C21" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B22" s="35">
         <v>0.01</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="9">
+        <v>-2.9382799999999998</v>
+      </c>
       <c r="E22" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="47"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="47">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" s="35">
         <v>0.05</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="9">
+        <v>-1.2431639999999999</v>
+      </c>
       <c r="E23" t="s">
         <v>65</v>
       </c>
-      <c r="F23" s="48"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F23" s="48">
+        <v>912</v>
+      </c>
+      <c r="I23" s="35"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B24" s="35">
         <v>0.1</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="9">
+        <v>-0.64895800000000003</v>
+      </c>
       <c r="F24" s="28"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="I24" s="35"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B25" s="35">
         <v>0.25</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="9">
+        <v>-9.5295599999999994E-2</v>
+      </c>
       <c r="E25" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="28"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="28">
+        <v>0.3211851</v>
+      </c>
+      <c r="I25" s="35"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="E26" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="28"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F26" s="28">
+        <v>1.20275</v>
+      </c>
+      <c r="I26" s="35"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B27" s="35">
         <v>0.5</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="9">
+        <v>0.1865655</v>
+      </c>
       <c r="F27" s="28"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="E28" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="28"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F28" s="28">
+        <v>1.446607</v>
+      </c>
+      <c r="I28" s="35"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B29" s="35">
         <v>0.75</v>
       </c>
-      <c r="C29" s="9"/>
+      <c r="C29" s="9">
+        <v>0.57733040000000002</v>
+      </c>
       <c r="E29" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="28"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F29" s="28">
+        <v>1.274227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="35">
         <v>0.9</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="9">
+        <v>1.4211590000000001</v>
+      </c>
       <c r="E30" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="49"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F30" s="49">
+        <v>9.5781530000000004</v>
+      </c>
+      <c r="I30" s="35"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B31" s="35">
         <v>0.95</v>
       </c>
-      <c r="C31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C31" s="9">
+        <v>2.3540019999999999</v>
+      </c>
+      <c r="I31" s="35"/>
+    </row>
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="45">
         <v>0.99</v>
       </c>
-      <c r="C32" s="46"/>
-    </row>
-    <row r="33" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="C32" s="46">
+        <v>5.2469239999999999</v>
+      </c>
+      <c r="I32" s="35"/>
+    </row>
+    <row r="33" spans="9:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I33" s="35"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4254,12 +4432,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4458,8 +4636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F0097E-5ADA-4F9F-8E43-EFEAF7A70026}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4482,14 +4660,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="66" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="92" t="s">
         <v>73</v>
       </c>
       <c r="B4" t="s">
@@ -4500,7 +4678,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="92" t="s">
         <v>72</v>
       </c>
       <c r="B5" t="s">
@@ -4511,7 +4689,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="92" t="s">
         <v>41</v>
       </c>
       <c r="B6" t="s">
@@ -4522,12 +4700,12 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="67" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="92" t="s">
         <v>81</v>
       </c>
       <c r="B8" t="s">
@@ -4538,7 +4716,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="92" t="s">
         <v>47</v>
       </c>
       <c r="B9" t="s">
@@ -4549,7 +4727,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="92" t="s">
         <v>82</v>
       </c>
       <c r="B10" t="s">
@@ -4560,7 +4738,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="92" t="s">
         <v>83</v>
       </c>
       <c r="B11" t="s">
@@ -4571,7 +4749,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="92" t="s">
         <v>50</v>
       </c>
       <c r="B12" t="s">
@@ -4582,7 +4760,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="92" t="s">
         <v>51</v>
       </c>
       <c r="B13" t="s">
@@ -4593,12 +4771,12 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="67" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="92" t="s">
         <v>79</v>
       </c>
       <c r="B15" t="s">
@@ -4609,7 +4787,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="92" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
@@ -4620,7 +4798,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="92" t="s">
         <v>44</v>
       </c>
       <c r="B17" t="s">
@@ -4631,7 +4809,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="92" t="s">
         <v>80</v>
       </c>
       <c r="B18" t="s">
@@ -4642,12 +4820,12 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="67" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="92" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="s">
@@ -4658,7 +4836,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="92" t="s">
         <v>53</v>
       </c>
       <c r="B21" t="s">
@@ -4669,7 +4847,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="92" t="s">
         <v>74</v>
       </c>
       <c r="B22" t="s">
@@ -4680,7 +4858,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="92" t="s">
         <v>75</v>
       </c>
       <c r="B23" t="s">
@@ -4691,7 +4869,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="92" t="s">
         <v>76</v>
       </c>
       <c r="B24" t="s">
@@ -4702,7 +4880,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="92" t="s">
         <v>77</v>
       </c>
       <c r="B25" t="s">
@@ -4713,7 +4891,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="92" t="s">
         <v>58</v>
       </c>
       <c r="B26" t="s">
@@ -4724,7 +4902,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="93" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="41" t="s">
@@ -4748,7 +4926,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="B5:C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -4823,66 +5001,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="79" t="s">
+      <c r="H1" s="77" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="N1" s="79" t="s">
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="N1" s="77" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="T1" s="79" t="s">
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="T1" s="77" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="80" t="s">
+      <c r="H2" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="N2" s="80" t="s">
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="N2" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="T2" s="80" t="s">
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="T2" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="81"/>
-      <c r="X2" s="81"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -5553,13 +5731,13 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="71" t="s">
+      <c r="I18" s="69" t="s">
         <v>249</v>
       </c>
-      <c r="J18" s="71" t="s">
+      <c r="J18" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="K18" s="71" t="s">
+      <c r="K18" s="69" t="s">
         <v>250</v>
       </c>
       <c r="L18" s="4"/>
@@ -5633,13 +5811,13 @@
       </c>
       <c r="G21" s="58"/>
       <c r="H21" s="58"/>
-      <c r="I21" s="72" t="s">
+      <c r="I21" s="70" t="s">
         <v>245</v>
       </c>
       <c r="J21" s="56">
         <v>93</v>
       </c>
-      <c r="K21" s="72">
+      <c r="K21" s="70">
         <f>+R7/F7</f>
         <v>0.82843257638348444</v>
       </c>
@@ -5827,16 +6005,16 @@
       <c r="B30" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="70">
+      <c r="C30" s="68">
         <v>0.2790882670355333</v>
       </c>
-      <c r="D30" s="70">
+      <c r="D30" s="68">
         <v>0.32358687319242407</v>
       </c>
-      <c r="E30" s="70">
+      <c r="E30" s="68">
         <v>0.41088869394235378</v>
       </c>
-      <c r="F30" s="70">
+      <c r="F30" s="68">
         <v>0.44647090411330181</v>
       </c>
       <c r="G30" s="28"/>
@@ -5901,10 +6079,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DD79C6-8E03-4472-BA01-B1AB9175E2E7}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
   <dimension ref="B2:C65"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5914,10 +6095,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="80" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="82"/>
+      <c r="C2" s="80"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -6441,8 +6622,8 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:D42"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6452,13 +6633,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6572,12 +6753,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="84" t="s">
+      <c r="A10" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -6876,12 +7057,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="84" t="s">
+      <c r="A37" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="84"/>
-      <c r="C37" s="84"/>
-      <c r="D37" s="84"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -7196,7 +7377,7 @@
   </sheetPr>
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A21" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -7215,13 +7396,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -7459,13 +7640,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -7493,13 +7674,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="85" t="s">
+      <c r="A25" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="85"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -7761,13 +7942,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="86" t="s">
+      <c r="A43" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="86"/>
-      <c r="C43" s="86"/>
-      <c r="D43" s="86"/>
-      <c r="E43" s="86"/>
+      <c r="B43" s="84"/>
+      <c r="C43" s="84"/>
+      <c r="D43" s="84"/>
+      <c r="E43" s="84"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -8135,36 +8316,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="87"/>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
-      <c r="Z3" s="87"/>
-      <c r="AA3" s="87"/>
-      <c r="AB3" s="87"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="85"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="85"/>
+      <c r="AB3" s="85"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -8648,35 +8829,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="91" t="s">
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="88" t="s">
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="89" t="s">
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="89"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="87"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>

<commit_message>
Added comparison of sigma estimates
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_7_6.xlsx
+++ b/results/tables/final_tables_7_6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312C4945-B38C-42C5-A737-43EE3720B6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43CD690-B346-4414-902B-F85466D3F7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-21840" windowWidth="38620" windowHeight="21100" tabRatio="656" activeTab="11" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" activeTab="11" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="291">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -956,6 +956,45 @@
   </si>
   <si>
     <t>Correlation index</t>
+  </si>
+  <si>
+    <t>Exclusive of 93 occ sample</t>
+  </si>
+  <si>
+    <t>Sample 62 occ</t>
+  </si>
+  <si>
+    <t>Sigma</t>
+  </si>
+  <si>
+    <t>&lt;=1</t>
+  </si>
+  <si>
+    <t>&gt;1</t>
+  </si>
+  <si>
+    <t>1239 mngers and prop. in other srvcs ne</t>
+  </si>
+  <si>
+    <t>3534 fin., invest, and taxation analyst</t>
+  </si>
+  <si>
+    <t>3537 finantial and accounting techs, an</t>
+  </si>
+  <si>
+    <t>6211 Leisure And Travel Service Occupat</t>
+  </si>
+  <si>
+    <t>8121 Plant and machine operatives</t>
+  </si>
+  <si>
+    <t>9211 post wrkr, mail sort, msngr, couri</t>
+  </si>
+  <si>
+    <t>9226 leisure and theme park attendants</t>
+  </si>
+  <si>
+    <t>List of occupation</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1362,6 +1401,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1401,18 +1449,13 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1600,6 +1643,55 @@
         <a:xfrm>
           <a:off x="6515099" y="11009491"/>
           <a:ext cx="6542286" cy="4755978"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>232896</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>98781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D00CF1E3-5AC5-5FBD-1DD9-177C7BF14F70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="349250" y="6032500"/>
+          <a:ext cx="13440896" cy="9877782"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1965,14 +2057,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="79" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
@@ -2074,14 +2166,14 @@
     </row>
     <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="79" t="s">
         <v>277</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
@@ -2210,20 +2302,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="90" t="s">
+      <c r="G2" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2466,11 +2558,11 @@
       <c r="B13" s="54">
         <v>62</v>
       </c>
-      <c r="G13" s="90" t="s">
+      <c r="G13" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G14" s="8" t="s">
@@ -2484,13 +2576,13 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="91" t="s">
+      <c r="A15" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
       <c r="G15" s="18">
         <f t="shared" ref="G15:I17" si="4">+C18/$B18</f>
         <v>2.2692799840412765</v>
@@ -2634,11 +2726,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="90" t="s">
+      <c r="G24" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="90"/>
-      <c r="I24" s="90"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -2664,13 +2756,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="91"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
+      <c r="B26" s="93"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
       <c r="G26" s="18">
         <f t="shared" ref="G26:I28" si="5">+C29/$B29</f>
         <v>1.0840988998256753</v>
@@ -2847,20 +2939,20 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="91" t="s">
+      <c r="A37" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="91"/>
-      <c r="C37" s="91"/>
-      <c r="D37" s="91"/>
-      <c r="E37" s="91"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="93"/>
+      <c r="D37" s="93"/>
+      <c r="E37" s="93"/>
     </row>
     <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="90" t="s">
+      <c r="G38" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="90"/>
-      <c r="I38" s="90"/>
+      <c r="H38" s="79"/>
+      <c r="I38" s="79"/>
     </row>
     <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -3118,20 +3210,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A51" s="91" t="s">
+      <c r="A51" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="91"/>
-      <c r="C51" s="91"/>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
+      <c r="B51" s="93"/>
+      <c r="C51" s="93"/>
+      <c r="D51" s="93"/>
+      <c r="E51" s="93"/>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="90" t="s">
+      <c r="G52" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="90"/>
-      <c r="I52" s="90"/>
+      <c r="H52" s="79"/>
+      <c r="I52" s="79"/>
     </row>
     <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -3292,6 +3384,16 @@
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="G24:I24"/>
   </mergeCells>
+  <conditionalFormatting sqref="G4:G6">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G15:G17">
     <cfRule type="colorScale" priority="15">
       <colorScale>
@@ -3299,6 +3401,46 @@
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26:G28">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40:G43 G45">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G54:G56">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H6">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -3312,48 +3454,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15:I17">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G6">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H6">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I6">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G40:G43 G45">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="H26:H28">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3372,6 +3474,46 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H54:H56">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I6">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:I17">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26:I28">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I40:I43 I45">
     <cfRule type="colorScale" priority="7">
       <colorScale>
@@ -3382,58 +3524,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G54:G56">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H54:H56">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I54:I56">
     <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G26:G28">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26:H28">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26:I28">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3474,20 +3566,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="90" t="s">
+      <c r="G4" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -3665,10 +3757,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3679,6 +3771,7 @@
     <col min="5" max="5" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.36328125" customWidth="1"/>
+    <col min="12" max="12" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -3859,7 +3952,7 @@
     <row r="16" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="L16" s="35"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>140</v>
       </c>
@@ -3868,7 +3961,7 @@
       </c>
       <c r="L17" s="35"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
@@ -3884,12 +3977,21 @@
       <c r="E18" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="83"/>
       <c r="L18" s="35"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K19" t="s">
+        <v>290</v>
+      </c>
+      <c r="O19" s="95"/>
+      <c r="P19" s="83" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q19" s="83"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="40"/>
       <c r="C20" s="10" t="s">
         <v>63</v>
@@ -3904,16 +4006,27 @@
         <v>129</v>
       </c>
       <c r="I20" s="5">
-        <v>80</v>
+        <f>+I23-I21</f>
+        <v>86</v>
+      </c>
+      <c r="K20" t="s">
+        <v>283</v>
       </c>
       <c r="L20" s="35"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="O20" s="23"/>
+      <c r="P20" s="94" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q20" s="94" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B21" s="35">
         <v>0.01</v>
       </c>
       <c r="C21" s="9">
-        <v>-166.69640000000001</v>
+        <v>-4.8694680000000004</v>
       </c>
       <c r="E21" t="s">
         <v>65</v>
@@ -3925,31 +4038,54 @@
         <v>130</v>
       </c>
       <c r="I21">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="K21" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="O21" s="95" t="s">
+        <v>278</v>
+      </c>
+      <c r="P21">
+        <v>28</v>
+      </c>
+      <c r="Q21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B22" s="35">
         <v>0.05</v>
       </c>
       <c r="C22" s="9">
-        <v>-14.417479999999999</v>
+        <v>-2.0304549999999999</v>
       </c>
       <c r="F22" s="28"/>
-      <c r="L22" s="35"/>
-    </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K22" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="O22" s="95" t="s">
+        <v>279</v>
+      </c>
+      <c r="P22">
+        <v>58</v>
+      </c>
+      <c r="Q22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="35">
         <v>0.1</v>
       </c>
       <c r="C23" s="9">
-        <v>-4.6349489999999998</v>
+        <v>-0.63951970000000002</v>
       </c>
       <c r="E23" t="s">
         <v>66</v>
       </c>
       <c r="F23" s="28">
-        <v>1.2513000000000001</v>
+        <v>-1.32762E-2</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>71</v>
@@ -3957,95 +4093,133 @@
       <c r="I23" s="19">
         <v>93</v>
       </c>
-      <c r="L23" s="35"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K23" s="35" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B24" s="35">
         <v>0.25</v>
       </c>
       <c r="C24" s="9">
-        <v>-1.3360289999999999</v>
+        <v>-0.1918347</v>
       </c>
       <c r="E24" t="s">
         <v>67</v>
       </c>
       <c r="F24" s="28">
-        <v>23.260300000000001</v>
-      </c>
-      <c r="L24" s="35"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1.168353</v>
+      </c>
+      <c r="K24" s="35" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="F25" s="28"/>
-      <c r="L25" s="35"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B26" s="35">
         <v>0.5</v>
       </c>
       <c r="C26" s="9">
-        <v>0.63808260000000006</v>
+        <v>1.5392599999999999E-2</v>
       </c>
       <c r="E26" t="s">
         <v>68</v>
       </c>
       <c r="F26" s="28">
-        <v>541.04150000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1.365048</v>
+      </c>
+      <c r="K26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="E27" t="s">
         <v>69</v>
       </c>
       <c r="F27" s="28">
-        <v>-3.6497830000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>-0.3439432</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="35">
         <v>0.75</v>
       </c>
       <c r="C28" s="9">
-        <v>4.7886990000000003</v>
+        <v>0.36161979999999999</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>70</v>
       </c>
       <c r="F28" s="49">
-        <v>33.000590000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+        <v>13.51919</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B29" s="35">
         <v>0.9</v>
       </c>
       <c r="C29" s="9">
-        <v>15.169890000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0.87319409999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B30" s="35">
         <v>0.95</v>
       </c>
       <c r="C30" s="9">
-        <v>31.69042</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>1.177781</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="45">
         <v>0.99</v>
       </c>
       <c r="C31" s="46">
-        <v>87.77825</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>5.731446</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="E32" s="35"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E33" s="35"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E34" s="35"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E35" s="35"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E37" s="35"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E39" s="35"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E40" s="35"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E41" s="35"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E42" s="35"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="H18:I18"/>
+    <mergeCell ref="P19:Q19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4432,12 +4606,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4667,7 +4841,7 @@
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="77" t="s">
         <v>73</v>
       </c>
       <c r="B4" t="s">
@@ -4678,7 +4852,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="77" t="s">
         <v>72</v>
       </c>
       <c r="B5" t="s">
@@ -4689,7 +4863,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="77" t="s">
         <v>41</v>
       </c>
       <c r="B6" t="s">
@@ -4705,7 +4879,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="92" t="s">
+      <c r="A8" s="77" t="s">
         <v>81</v>
       </c>
       <c r="B8" t="s">
@@ -4716,7 +4890,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="92" t="s">
+      <c r="A9" s="77" t="s">
         <v>47</v>
       </c>
       <c r="B9" t="s">
@@ -4727,7 +4901,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="92" t="s">
+      <c r="A10" s="77" t="s">
         <v>82</v>
       </c>
       <c r="B10" t="s">
@@ -4738,7 +4912,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="92" t="s">
+      <c r="A11" s="77" t="s">
         <v>83</v>
       </c>
       <c r="B11" t="s">
@@ -4749,7 +4923,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="92" t="s">
+      <c r="A12" s="77" t="s">
         <v>50</v>
       </c>
       <c r="B12" t="s">
@@ -4760,7 +4934,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="92" t="s">
+      <c r="A13" s="77" t="s">
         <v>51</v>
       </c>
       <c r="B13" t="s">
@@ -4776,7 +4950,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="92" t="s">
+      <c r="A15" s="77" t="s">
         <v>79</v>
       </c>
       <c r="B15" t="s">
@@ -4787,7 +4961,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="77" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
@@ -4798,7 +4972,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="92" t="s">
+      <c r="A17" s="77" t="s">
         <v>44</v>
       </c>
       <c r="B17" t="s">
@@ -4809,7 +4983,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="92" t="s">
+      <c r="A18" s="77" t="s">
         <v>80</v>
       </c>
       <c r="B18" t="s">
@@ -4825,7 +4999,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="92" t="s">
+      <c r="A20" s="77" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="s">
@@ -4836,7 +5010,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="92" t="s">
+      <c r="A21" s="77" t="s">
         <v>53</v>
       </c>
       <c r="B21" t="s">
@@ -4847,7 +5021,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="92" t="s">
+      <c r="A22" s="77" t="s">
         <v>74</v>
       </c>
       <c r="B22" t="s">
@@ -4858,7 +5032,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="77" t="s">
         <v>75</v>
       </c>
       <c r="B23" t="s">
@@ -4869,7 +5043,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="92" t="s">
+      <c r="A24" s="77" t="s">
         <v>76</v>
       </c>
       <c r="B24" t="s">
@@ -4880,7 +5054,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="77" t="s">
         <v>77</v>
       </c>
       <c r="B25" t="s">
@@ -4891,7 +5065,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="92" t="s">
+      <c r="A26" s="77" t="s">
         <v>58</v>
       </c>
       <c r="B26" t="s">
@@ -4902,7 +5076,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="93" t="s">
+      <c r="A27" s="78" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="41" t="s">
@@ -5001,66 +5175,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="80" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="80" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="N1" s="77" t="s">
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="N1" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="T1" s="77" t="s">
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="T1" s="80" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="78" t="s">
+      <c r="H2" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="N2" s="78" t="s">
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="N2" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="T2" s="78" t="s">
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="T2" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="82"/>
+      <c r="W2" s="82"/>
+      <c r="X2" s="82"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -6095,10 +6269,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="83" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="80"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -6633,13 +6807,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6753,12 +6927,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -7057,12 +7231,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="82" t="s">
+      <c r="A37" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="82"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -7396,13 +7570,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -7640,13 +7814,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="84" t="s">
+      <c r="A21" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -7674,13 +7848,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="83" t="s">
+      <c r="A25" s="86" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -7942,13 +8116,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="84" t="s">
+      <c r="A43" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="84"/>
-      <c r="C43" s="84"/>
-      <c r="D43" s="84"/>
-      <c r="E43" s="84"/>
+      <c r="B43" s="87"/>
+      <c r="C43" s="87"/>
+      <c r="D43" s="87"/>
+      <c r="E43" s="87"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -8316,36 +8490,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="85"/>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="85"/>
-      <c r="Y3" s="85"/>
-      <c r="Z3" s="85"/>
-      <c r="AA3" s="85"/>
-      <c r="AB3" s="85"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="88"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="88"/>
+      <c r="T3" s="88"/>
+      <c r="U3" s="88"/>
+      <c r="V3" s="88"/>
+      <c r="W3" s="88"/>
+      <c r="X3" s="88"/>
+      <c r="Y3" s="88"/>
+      <c r="Z3" s="88"/>
+      <c r="AA3" s="88"/>
+      <c r="AB3" s="88"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -8829,35 +9003,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="89" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="86" t="s">
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87" t="s">
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="87"/>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="87"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="90"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>

<commit_message>
added same manual 3eq results
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_7_6.xlsx
+++ b/results/tables/final_tables_7_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43CD690-B346-4414-902B-F85466D3F7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8793C042-778B-477D-803B-15A2B90C5CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" activeTab="11" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="7" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -1007,7 +1007,7 @@
     <numFmt numFmtId="166" formatCode="0.0000_);\(0.0000\)"/>
     <numFmt numFmtId="167" formatCode="0.000_);\(0.000\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1089,8 +1089,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1148,6 +1155,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1253,7 +1266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1400,13 +1413,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1452,10 +1468,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="11" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2057,14 +2073,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
@@ -2166,14 +2182,14 @@
     </row>
     <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="80" t="s">
         <v>277</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
@@ -2291,8 +2307,8 @@
   </sheetPr>
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2301,23 +2317,23 @@
     <col min="2" max="5" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="93" t="s">
+    <row r="1" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="79" t="s">
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G2" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -2342,8 +2358,20 @@
       <c r="I3" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K3" s="95">
+        <v>2.3825693796604801E-2</v>
+      </c>
+      <c r="L3" s="95">
+        <v>8.6462761603051996E-2</v>
+      </c>
+      <c r="M3" s="95">
+        <v>9.1086936740078506E-2</v>
+      </c>
+      <c r="N3" s="95">
+        <v>9.1114556856590104E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -2371,23 +2399,35 @@
         <f t="shared" si="0"/>
         <v>1.0266230598457746</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K4" s="95">
+        <v>2.3825693796604801E-2</v>
+      </c>
+      <c r="L4" s="95">
+        <v>0.102623074984331</v>
+      </c>
+      <c r="M4" s="95">
+        <v>9.9970167180033806E-2</v>
+      </c>
+      <c r="N4" s="95">
+        <v>0.131180946644253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" s="73">
-        <f>-G8</f>
-        <v>-4.0630067214601502E-2</v>
+        <f>+K7</f>
+        <v>-2.3825693796604801E-2</v>
       </c>
       <c r="C5" s="73">
-        <f t="shared" ref="C5:E5" si="1">-H8</f>
-        <v>-8.3571611908693402E-2</v>
+        <f t="shared" ref="C5:E5" si="1">+L7</f>
+        <v>-8.6462761603051996E-2</v>
       </c>
       <c r="D5" s="73">
         <f t="shared" si="1"/>
-        <v>-9.7324360517554401E-2</v>
+        <v>-9.1086936740078506E-2</v>
       </c>
       <c r="E5" s="73">
         <f t="shared" si="1"/>
-        <v>-9.1894583020425705E-2</v>
+        <v>-9.1114556856590104E-2</v>
       </c>
       <c r="G5" s="18">
         <f>+C6/$B6</f>
@@ -2401,8 +2441,20 @@
         <f>+E6/$B6</f>
         <v>0.13736843489130302</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K5" s="95">
+        <v>2.3825693796604801E-2</v>
+      </c>
+      <c r="L5" s="95">
+        <v>8.7913295104061095E-2</v>
+      </c>
+      <c r="M5" s="95">
+        <v>9.5241393813421102E-2</v>
+      </c>
+      <c r="N5" s="95">
+        <v>7.0074395414781599E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2431,25 +2483,41 @@
         <v>0.35047134189088008</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B7" s="73">
-        <f>+-G9</f>
-        <v>-3.6007782107965597E-2</v>
+        <f>+K8</f>
+        <v>-2.3825693796604801E-2</v>
       </c>
       <c r="C7" s="73">
-        <f t="shared" ref="C7:E7" si="2">+-H9</f>
-        <v>-0.106732211233662</v>
+        <f t="shared" ref="C7:E7" si="2">+L8</f>
+        <v>-0.102623074984331</v>
       </c>
       <c r="D7" s="73">
         <f t="shared" si="2"/>
-        <v>-9.9568615714996894E-2</v>
+        <v>-9.9970167180033806E-2</v>
       </c>
       <c r="E7" s="73">
         <f t="shared" si="2"/>
-        <v>-0.124123017797548</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>-0.131180946644253</v>
+      </c>
+      <c r="K7" s="95">
+        <f>-K3</f>
+        <v>-2.3825693796604801E-2</v>
+      </c>
+      <c r="L7" s="95">
+        <f t="shared" ref="L7:N7" si="3">-L3</f>
+        <v>-8.6462761603051996E-2</v>
+      </c>
+      <c r="M7" s="95">
+        <f t="shared" si="3"/>
+        <v>-9.1086936740078506E-2</v>
+      </c>
+      <c r="N7" s="95">
+        <f t="shared" si="3"/>
+        <v>-9.1114556856590104E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2465,76 +2533,108 @@
       <c r="E8" s="72">
         <v>8.8865355218595204E-2</v>
       </c>
-      <c r="G8" s="75">
-        <v>4.0630067214601502E-2</v>
-      </c>
-      <c r="H8" s="75">
-        <v>8.3571611908693402E-2</v>
-      </c>
-      <c r="I8" s="75">
-        <v>9.7324360517554401E-2</v>
+      <c r="G8" s="95">
+        <v>0.250506013088374</v>
+      </c>
+      <c r="H8" s="95">
+        <v>0.27695568077675098</v>
+      </c>
+      <c r="I8" s="95">
+        <v>0.83798797041589701</v>
       </c>
       <c r="J8" s="75">
-        <v>9.1894583020425705E-2</v>
-      </c>
-      <c r="K8" s="75"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.26330301045276699</v>
+      </c>
+      <c r="K8" s="95">
+        <f t="shared" ref="K8:N8" si="4">-K4</f>
+        <v>-2.3825693796604801E-2</v>
+      </c>
+      <c r="L8" s="95">
+        <f t="shared" si="4"/>
+        <v>-0.102623074984331</v>
+      </c>
+      <c r="M8" s="95">
+        <f t="shared" si="4"/>
+        <v>-9.9970167180033806E-2</v>
+      </c>
+      <c r="N8" s="95">
+        <f t="shared" si="4"/>
+        <v>-0.131180946644253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19"/>
       <c r="B9" s="74">
-        <f>-G10</f>
-        <v>-3.4757427098277102E-2</v>
+        <f>+K9</f>
+        <v>-2.3825693796604801E-2</v>
       </c>
       <c r="C9" s="74">
-        <f t="shared" ref="C9:E9" si="3">-H10</f>
-        <v>-9.6253137771482297E-2</v>
+        <f t="shared" ref="C9:E9" si="5">+L9</f>
+        <v>-8.7913295104061095E-2</v>
       </c>
       <c r="D9" s="74">
-        <f t="shared" si="3"/>
-        <v>-0.102214538826463</v>
+        <f t="shared" si="5"/>
+        <v>-9.5241393813421102E-2</v>
       </c>
       <c r="E9" s="74">
-        <f t="shared" si="3"/>
-        <v>-7.0983830304353304E-2</v>
-      </c>
-      <c r="G9" s="75">
-        <v>3.6007782107965597E-2</v>
-      </c>
-      <c r="H9" s="75">
-        <v>0.106732211233662</v>
-      </c>
-      <c r="I9" s="75">
-        <v>9.9568615714996894E-2</v>
+        <f t="shared" si="5"/>
+        <v>-7.0074395414781599E-3</v>
+      </c>
+      <c r="G9" s="95">
+        <v>0.250506013088374</v>
+      </c>
+      <c r="H9" s="95">
+        <v>0.489870693201512</v>
+      </c>
+      <c r="I9" s="95">
+        <v>0.77794346839460005</v>
       </c>
       <c r="J9" s="75">
-        <v>0.124123017797548</v>
-      </c>
-      <c r="K9" s="75"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G10" s="75">
-        <v>3.4757427098277102E-2</v>
-      </c>
-      <c r="H10" s="75">
-        <v>9.6253137771482297E-2</v>
-      </c>
-      <c r="I10" s="75">
-        <v>0.102214538826463</v>
+        <v>2.3903857171145598E-2</v>
+      </c>
+      <c r="K9" s="95">
+        <f t="shared" ref="K9:N9" si="6">-K5</f>
+        <v>-2.3825693796604801E-2</v>
+      </c>
+      <c r="L9" s="95">
+        <f t="shared" si="6"/>
+        <v>-8.7913295104061095E-2</v>
+      </c>
+      <c r="M9" s="95">
+        <f t="shared" si="6"/>
+        <v>-9.5241393813421102E-2</v>
+      </c>
+      <c r="N9" s="95">
+        <f t="shared" si="6"/>
+        <v>-7.0074395414781599E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G10" s="95">
+        <v>0.250506013088374</v>
+      </c>
+      <c r="H10" s="95">
+        <v>1.0339386129405901</v>
+      </c>
+      <c r="I10" s="95">
+        <v>0.127777976759439</v>
       </c>
       <c r="J10" s="75">
-        <v>7.0983830304353304E-2</v>
-      </c>
-      <c r="K10" s="75"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>8.5955322866406697E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B11" s="54" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="96"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
@@ -2551,20 +2651,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B13" s="54">
         <v>62</v>
       </c>
-      <c r="G13" s="79" t="s">
+      <c r="G13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G14" s="8" t="s">
         <v>4</v>
       </c>
@@ -2575,38 +2675,38 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="93" t="s">
+    <row r="15" spans="1:14" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
       <c r="G15" s="18">
-        <f t="shared" ref="G15:I17" si="4">+C18/$B18</f>
+        <f t="shared" ref="G15:I17" si="7">+C18/$B18</f>
         <v>2.2692799840412765</v>
       </c>
       <c r="H15" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.389518623297354</v>
       </c>
       <c r="I15" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.0096069126124061E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G16" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.4104194790539126</v>
       </c>
       <c r="H16" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.1527236641653915</v>
       </c>
       <c r="I16" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.2404717945099751E-2</v>
       </c>
     </row>
@@ -2627,15 +2727,15 @@
         <v>6</v>
       </c>
       <c r="G17" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.952135105688277</v>
       </c>
       <c r="H17" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.4224332808744315</v>
       </c>
       <c r="I17" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.992433008205325E-2</v>
       </c>
     </row>
@@ -2726,11 +2826,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="79" t="s">
+      <c r="G24" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -2756,23 +2856,23 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="93" t="s">
+      <c r="A26" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="93"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="93"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
+      <c r="E26" s="94"/>
       <c r="G26" s="18">
-        <f t="shared" ref="G26:I28" si="5">+C29/$B29</f>
+        <f t="shared" ref="G26:I28" si="8">+C29/$B29</f>
         <v>1.0840988998256753</v>
       </c>
       <c r="H26" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.7002892687797702</v>
       </c>
       <c r="I26" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.85609510095769148</v>
       </c>
       <c r="L26">
@@ -2790,15 +2890,15 @@
     </row>
     <row r="27" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G27" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.2651573917720484</v>
       </c>
       <c r="H27" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.6005843591077697</v>
       </c>
       <c r="I27" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.16090197814497112</v>
       </c>
       <c r="L27">
@@ -2831,15 +2931,15 @@
         <v>6</v>
       </c>
       <c r="G28" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.1755689228525847</v>
       </c>
       <c r="H28" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.63094595006553655</v>
       </c>
       <c r="I28" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.38561453292854309</v>
       </c>
     </row>
@@ -2939,20 +3039,20 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="93" t="s">
+      <c r="A37" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="93"/>
-      <c r="C37" s="93"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="93"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
     </row>
     <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="79" t="s">
+      <c r="G38" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="79"/>
-      <c r="I38" s="79"/>
+      <c r="H38" s="80"/>
+      <c r="I38" s="80"/>
     </row>
     <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -3016,15 +3116,15 @@
         <v>-3.27791808747964E-2</v>
       </c>
       <c r="C41" s="73">
-        <f t="shared" ref="C41:E41" si="6">-H45</f>
+        <f t="shared" ref="C41:E41" si="9">-H45</f>
         <v>-7.5396741976460305E-2</v>
       </c>
       <c r="D41" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-0.115293505002319</v>
       </c>
       <c r="E41" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-0.14196233908585501</v>
       </c>
       <c r="F41" s="18"/>
@@ -3077,20 +3177,22 @@
         <v>-3.5902339137002803E-2</v>
       </c>
       <c r="C43" s="73">
-        <f t="shared" ref="C43:E43" si="7">-H46</f>
+        <f t="shared" ref="C43:E43" si="10">-H46</f>
         <v>-8.7285450730600303E-2</v>
       </c>
       <c r="D43" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-8.3582228841739506E-2</v>
       </c>
       <c r="E43" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-9.8175524348070906E-2</v>
       </c>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
+      <c r="F43" s="96"/>
+      <c r="G43" s="97"/>
+      <c r="H43" s="97"/>
+      <c r="I43" s="97"/>
+      <c r="J43" s="96"/>
       <c r="K43" s="75"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
@@ -3109,6 +3211,11 @@
       <c r="E44" s="72">
         <v>4.5849482279728501E-2</v>
       </c>
+      <c r="F44" s="96"/>
+      <c r="G44" s="96"/>
+      <c r="H44" s="96"/>
+      <c r="I44" s="96"/>
+      <c r="J44" s="96"/>
       <c r="K44" s="75"/>
     </row>
     <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3118,42 +3225,44 @@
         <v>-3.5398027084865398E-2</v>
       </c>
       <c r="C45" s="74">
-        <f t="shared" ref="C45:E45" si="8">-H47</f>
+        <f t="shared" ref="C45:E45" si="11">-H47</f>
         <v>-8.8625088080741696E-2</v>
       </c>
       <c r="D45" s="74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-8.7677991056143698E-2</v>
       </c>
       <c r="E45" s="74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-7.5233432632621805E-2</v>
       </c>
-      <c r="G45" s="76">
+      <c r="F45" s="96"/>
+      <c r="G45" s="98">
         <v>3.27791808747964E-2</v>
       </c>
-      <c r="H45" s="76">
+      <c r="H45" s="98">
         <v>7.5396741976460305E-2</v>
       </c>
-      <c r="I45" s="76">
+      <c r="I45" s="98">
         <v>0.115293505002319</v>
       </c>
-      <c r="J45" s="75">
+      <c r="J45" s="95">
         <v>0.14196233908585501</v>
       </c>
       <c r="K45" s="75"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G46" s="75">
+      <c r="F46" s="96"/>
+      <c r="G46" s="95">
         <v>3.5902339137002803E-2</v>
       </c>
-      <c r="H46" s="75">
+      <c r="H46" s="95">
         <v>8.7285450730600303E-2</v>
       </c>
-      <c r="I46" s="75">
+      <c r="I46" s="95">
         <v>8.3582228841739506E-2</v>
       </c>
-      <c r="J46" s="75">
+      <c r="J46" s="95">
         <v>9.8175524348070906E-2</v>
       </c>
     </row>
@@ -3164,16 +3273,17 @@
       <c r="B47" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="G47" s="75">
+      <c r="F47" s="96"/>
+      <c r="G47" s="95">
         <v>3.5398027084865398E-2</v>
       </c>
-      <c r="H47" s="75">
+      <c r="H47" s="95">
         <v>8.8625088080741696E-2</v>
       </c>
-      <c r="I47" s="75">
+      <c r="I47" s="95">
         <v>8.7677991056143698E-2</v>
       </c>
-      <c r="J47" s="75">
+      <c r="J47" s="95">
         <v>7.5233432632621805E-2</v>
       </c>
     </row>
@@ -3210,20 +3320,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A51" s="93" t="s">
+      <c r="A51" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="93"/>
-      <c r="C51" s="93"/>
-      <c r="D51" s="93"/>
-      <c r="E51" s="93"/>
+      <c r="B51" s="94"/>
+      <c r="C51" s="94"/>
+      <c r="D51" s="94"/>
+      <c r="E51" s="94"/>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="79" t="s">
+      <c r="G52" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="79"/>
-      <c r="I52" s="79"/>
+      <c r="H52" s="80"/>
+      <c r="I52" s="80"/>
     </row>
     <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -3268,15 +3378,15 @@
         <v>0.15027534446115601</v>
       </c>
       <c r="G54" s="18">
-        <f t="shared" ref="G54:G56" si="9">+C54/$B54</f>
+        <f t="shared" ref="G54:G56" si="12">+C54/$B54</f>
         <v>1.373671978812486</v>
       </c>
       <c r="H54" s="18">
-        <f t="shared" ref="H54:H56" si="10">+D54/$B54</f>
+        <f t="shared" ref="H54:H56" si="13">+D54/$B54</f>
         <v>2.882317701442024</v>
       </c>
       <c r="I54" s="18">
-        <f t="shared" ref="I54:I56" si="11">+E54/$B54</f>
+        <f t="shared" ref="I54:I56" si="14">+E54/$B54</f>
         <v>0.54826548178845746</v>
       </c>
     </row>
@@ -3297,15 +3407,15 @@
         <v>7.8971052048355805E-2</v>
       </c>
       <c r="G55" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2.1206583692359722</v>
       </c>
       <c r="H55" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.2750245955063209</v>
       </c>
       <c r="I55" s="18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.28811846716361922</v>
       </c>
     </row>
@@ -3326,15 +3436,15 @@
         <v>0.13010063352593601</v>
       </c>
       <c r="G56" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.8654374748940057</v>
       </c>
       <c r="H56" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.2505536369075858</v>
       </c>
       <c r="I56" s="18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.47465994356458474</v>
       </c>
     </row>
@@ -3566,20 +3676,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="79" t="s">
+      <c r="G4" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -3759,7 +3869,7 @@
   </sheetPr>
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -3977,19 +4087,19 @@
       <c r="E18" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="84"/>
       <c r="L18" s="35"/>
     </row>
     <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K19" t="s">
         <v>290</v>
       </c>
-      <c r="O19" s="95"/>
-      <c r="P19" s="83" t="s">
+      <c r="O19" s="79"/>
+      <c r="P19" s="84" t="s">
         <v>280</v>
       </c>
-      <c r="Q19" s="83"/>
+      <c r="Q19" s="84"/>
     </row>
     <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="40"/>
@@ -4014,10 +4124,10 @@
       </c>
       <c r="L20" s="35"/>
       <c r="O20" s="23"/>
-      <c r="P20" s="94" t="s">
+      <c r="P20" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="Q20" s="94" t="s">
+      <c r="Q20" s="78" t="s">
         <v>282</v>
       </c>
     </row>
@@ -4043,7 +4153,7 @@
       <c r="K21" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="O21" s="95" t="s">
+      <c r="O21" s="79" t="s">
         <v>278</v>
       </c>
       <c r="P21">
@@ -4064,7 +4174,7 @@
       <c r="K22" s="35" t="s">
         <v>285</v>
       </c>
-      <c r="O22" s="95" t="s">
+      <c r="O22" s="79" t="s">
         <v>279</v>
       </c>
       <c r="P22">
@@ -4606,12 +4716,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4841,7 +4951,7 @@
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="76" t="s">
         <v>73</v>
       </c>
       <c r="B4" t="s">
@@ -4852,7 +4962,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="76" t="s">
         <v>72</v>
       </c>
       <c r="B5" t="s">
@@ -4863,7 +4973,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="76" t="s">
         <v>41</v>
       </c>
       <c r="B6" t="s">
@@ -4879,7 +4989,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="76" t="s">
         <v>81</v>
       </c>
       <c r="B8" t="s">
@@ -4890,7 +5000,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="76" t="s">
         <v>47</v>
       </c>
       <c r="B9" t="s">
@@ -4901,7 +5011,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="76" t="s">
         <v>82</v>
       </c>
       <c r="B10" t="s">
@@ -4912,7 +5022,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="76" t="s">
         <v>83</v>
       </c>
       <c r="B11" t="s">
@@ -4923,7 +5033,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="76" t="s">
         <v>50</v>
       </c>
       <c r="B12" t="s">
@@ -4934,7 +5044,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="76" t="s">
         <v>51</v>
       </c>
       <c r="B13" t="s">
@@ -4950,7 +5060,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="76" t="s">
         <v>79</v>
       </c>
       <c r="B15" t="s">
@@ -4961,7 +5071,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="76" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
@@ -4972,7 +5082,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="76" t="s">
         <v>44</v>
       </c>
       <c r="B17" t="s">
@@ -4983,7 +5093,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="76" t="s">
         <v>80</v>
       </c>
       <c r="B18" t="s">
@@ -4999,7 +5109,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="76" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="s">
@@ -5010,7 +5120,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="76" t="s">
         <v>53</v>
       </c>
       <c r="B21" t="s">
@@ -5021,7 +5131,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="76" t="s">
         <v>74</v>
       </c>
       <c r="B22" t="s">
@@ -5032,7 +5142,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="76" t="s">
         <v>75</v>
       </c>
       <c r="B23" t="s">
@@ -5043,7 +5153,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="76" t="s">
         <v>76</v>
       </c>
       <c r="B24" t="s">
@@ -5054,7 +5164,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="76" t="s">
         <v>77</v>
       </c>
       <c r="B25" t="s">
@@ -5065,7 +5175,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="76" t="s">
         <v>58</v>
       </c>
       <c r="B26" t="s">
@@ -5076,7 +5186,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="77" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="41" t="s">
@@ -5155,8 +5265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CAF832-E4CD-4D78-919A-B2CAC1381075}">
   <dimension ref="B1:AA34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5175,66 +5285,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="81" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="80" t="s">
+      <c r="H1" s="81" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="N1" s="80" t="s">
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="N1" s="81" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="T1" s="80" t="s">
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="T1" s="81" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="80"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="80"/>
-      <c r="X1" s="80"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81"/>
+      <c r="X1" s="81"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="82" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="82" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="N2" s="81" t="s">
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="N2" s="82" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="T2" s="81" t="s">
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="T2" s="82" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="82"/>
-      <c r="V2" s="82"/>
-      <c r="W2" s="82"/>
-      <c r="X2" s="82"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -6269,10 +6379,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="84" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="83"/>
+      <c r="C2" s="84"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -6796,7 +6906,7 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -6807,13 +6917,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6927,12 +7037,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -7231,12 +7341,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="85" t="s">
+      <c r="A37" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="85"/>
-      <c r="C37" s="85"/>
-      <c r="D37" s="85"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -7570,13 +7680,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="87" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -7814,13 +7924,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="87" t="s">
+      <c r="A21" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="87"/>
-      <c r="C21" s="87"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -7848,13 +7958,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="86" t="s">
+      <c r="A25" s="87" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="86"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -8116,13 +8226,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="87" t="s">
+      <c r="A43" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="87"/>
-      <c r="C43" s="87"/>
-      <c r="D43" s="87"/>
-      <c r="E43" s="87"/>
+      <c r="B43" s="88"/>
+      <c r="C43" s="88"/>
+      <c r="D43" s="88"/>
+      <c r="E43" s="88"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -8490,36 +8600,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
-      <c r="Q3" s="88"/>
-      <c r="R3" s="88"/>
-      <c r="S3" s="88"/>
-      <c r="T3" s="88"/>
-      <c r="U3" s="88"/>
-      <c r="V3" s="88"/>
-      <c r="W3" s="88"/>
-      <c r="X3" s="88"/>
-      <c r="Y3" s="88"/>
-      <c r="Z3" s="88"/>
-      <c r="AA3" s="88"/>
-      <c r="AB3" s="88"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="89"/>
+      <c r="T3" s="89"/>
+      <c r="U3" s="89"/>
+      <c r="V3" s="89"/>
+      <c r="W3" s="89"/>
+      <c r="X3" s="89"/>
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="89"/>
+      <c r="AA3" s="89"/>
+      <c r="AB3" s="89"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -9003,35 +9113,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="92" t="s">
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="89" t="s">
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90" t="s">
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="90"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="91"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>

<commit_message>
Corrected same manual standard errors for 2eq
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_7_6.xlsx
+++ b/results/tables/final_tables_7_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226B7A7E-0C80-4D3A-8FBE-BB16FAE29258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F40AC45-6B09-48CF-AED8-84F6C9089331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="9" activeTab="11" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="7" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="291">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -951,6 +951,51 @@
   <si>
     <t>importance of: analysing complex problems in depth</t>
   </si>
+  <si>
+    <t>Welch index</t>
+  </si>
+  <si>
+    <t>Correlation index</t>
+  </si>
+  <si>
+    <t>Exclusive of 93 occ sample</t>
+  </si>
+  <si>
+    <t>Sample 62 occ</t>
+  </si>
+  <si>
+    <t>Sigma</t>
+  </si>
+  <si>
+    <t>&lt;=1</t>
+  </si>
+  <si>
+    <t>&gt;1</t>
+  </si>
+  <si>
+    <t>1239 mngers and prop. in other srvcs ne</t>
+  </si>
+  <si>
+    <t>3534 fin., invest, and taxation analyst</t>
+  </si>
+  <si>
+    <t>3537 finantial and accounting techs, an</t>
+  </si>
+  <si>
+    <t>6211 Leisure And Travel Service Occupat</t>
+  </si>
+  <si>
+    <t>8121 Plant and machine operatives</t>
+  </si>
+  <si>
+    <t>9211 post wrkr, mail sort, msngr, couri</t>
+  </si>
+  <si>
+    <t>9226 leisure and theme park attendants</t>
+  </si>
+  <si>
+    <t>List of occupation</t>
+  </si>
 </sst>
 </file>
 
@@ -962,7 +1007,7 @@
     <numFmt numFmtId="166" formatCode="0.0000_);\(0.0000\)"/>
     <numFmt numFmtId="167" formatCode="0.000_);\(0.000\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1044,8 +1089,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1103,6 +1155,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1208,7 +1266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1335,12 +1393,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1357,7 +1413,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="11" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1395,9 +1467,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1590,6 +1659,55 @@
         <a:xfrm>
           <a:off x="6515099" y="11009491"/>
           <a:ext cx="6542286" cy="4755978"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>232896</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>98781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D00CF1E3-5AC5-5FBD-1DD9-177C7BF14F70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="349250" y="6032500"/>
+          <a:ext cx="13440896" cy="9877782"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1938,119 +2056,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7471085D-BC16-46A9-AF3A-D1F9FAE30012}">
-  <dimension ref="A2:F9"/>
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="15.1796875" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="84" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>254</v>
       </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="18">
+        <v>0.99999998999999995</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B4" s="18">
-        <v>0.99999998999999995</v>
-      </c>
-      <c r="C4" s="18"/>
+        <v>0.78706158000000004</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1</v>
+      </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>252</v>
+        <v>93</v>
       </c>
       <c r="B5" s="18">
-        <v>0.78706158000000004</v>
+        <v>0.36120983000000001</v>
       </c>
       <c r="C5" s="18">
-        <v>1</v>
-      </c>
-      <c r="D5" s="18"/>
+        <v>0.47599598999999998</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.99999998999999995</v>
+      </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="18">
+        <v>-6.5339869999999994E-2</v>
+      </c>
+      <c r="C6" s="18">
+        <v>4.1870570000000003E-2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.37941629999999998</v>
+      </c>
+      <c r="E6" s="18">
+        <v>1</v>
+      </c>
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="71">
+        <v>-0.62474819000000004</v>
+      </c>
+      <c r="C7" s="71">
+        <v>-0.72046911000000002</v>
+      </c>
+      <c r="D7" s="71">
+        <v>-0.84169570999999999</v>
+      </c>
+      <c r="E7" s="71">
+        <v>-0.57978885999999996</v>
+      </c>
+      <c r="F7" s="71">
+        <v>0.99999998999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="84" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" s="84"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="18">
-        <v>0.36120983000000001</v>
-      </c>
-      <c r="C6" s="18">
-        <v>0.47599598999999998</v>
-      </c>
-      <c r="D6" s="18">
-        <v>0.99999998999999995</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="E10" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="B7" s="18">
-        <v>-6.5339869999999994E-2</v>
-      </c>
-      <c r="C7" s="18">
-        <v>4.1870570000000003E-2</v>
-      </c>
-      <c r="D7" s="18">
-        <v>0.37941629999999998</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="F10" s="10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="18">
         <v>1</v>
       </c>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="18">
+        <v>0.86419999999999997</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="18">
+        <v>0.65110000000000001</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0.80120000000000002</v>
+      </c>
+      <c r="D13" s="18">
+        <v>1</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="18">
+        <v>0.45619999999999999</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0.628</v>
+      </c>
+      <c r="D14" s="18">
+        <v>0.83679999999999999</v>
+      </c>
+      <c r="E14" s="18">
+        <v>1</v>
+      </c>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B8" s="73">
-        <v>-0.62474819000000004</v>
-      </c>
-      <c r="C8" s="73">
-        <v>-0.72046911000000002</v>
-      </c>
-      <c r="D8" s="73">
-        <v>-0.84169570999999999</v>
-      </c>
-      <c r="E8" s="73">
-        <v>-0.57978885999999996</v>
-      </c>
-      <c r="F8" s="73">
-        <v>0.99999998999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="B15" s="71">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="C15" s="71">
+        <v>0.17519999999999999</v>
+      </c>
+      <c r="D15" s="71">
+        <v>0.3337</v>
+      </c>
+      <c r="E15" s="71">
+        <v>0.39879999999999999</v>
+      </c>
+      <c r="F15" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A9:F9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2063,8 +2307,8 @@
   </sheetPr>
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2073,23 +2317,23 @@
     <col min="2" max="5" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="93" t="s">
+    <row r="1" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="92" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G2" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -2114,21 +2358,33 @@
       <c r="I3" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K3" s="80">
+        <v>2.3825693796604801E-2</v>
+      </c>
+      <c r="L3" s="80">
+        <v>8.6462761603051996E-2</v>
+      </c>
+      <c r="M3" s="80">
+        <v>9.1086936740078506E-2</v>
+      </c>
+      <c r="N3" s="80">
+        <v>9.1114556856590104E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="74">
+      <c r="B4" s="72">
         <v>0.25355954851870199</v>
       </c>
-      <c r="C4" s="74">
+      <c r="C4" s="72">
         <v>0.26387458982134598</v>
       </c>
-      <c r="D4" s="74">
+      <c r="D4" s="72">
         <v>0.85431293094579996</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="72">
         <v>0.26031007955338298</v>
       </c>
       <c r="G4" s="18">
@@ -2143,23 +2399,35 @@
         <f t="shared" si="0"/>
         <v>1.0266230598457746</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="75">
-        <f>-G8</f>
-        <v>-4.0630067214601502E-2</v>
-      </c>
-      <c r="C5" s="75">
-        <f t="shared" ref="C5:E5" si="1">-H8</f>
-        <v>-8.3571611908693402E-2</v>
-      </c>
-      <c r="D5" s="75">
+      <c r="K4" s="80">
+        <v>2.3825693796604801E-2</v>
+      </c>
+      <c r="L4" s="80">
+        <v>0.102623074984331</v>
+      </c>
+      <c r="M4" s="80">
+        <v>9.9970167180033806E-2</v>
+      </c>
+      <c r="N4" s="80">
+        <v>0.131180946644253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B5" s="73">
+        <f>+K7</f>
+        <v>-2.3825693796604801E-2</v>
+      </c>
+      <c r="C5" s="73">
+        <f t="shared" ref="C5:E5" si="1">+L7</f>
+        <v>-8.6462761603051996E-2</v>
+      </c>
+      <c r="D5" s="73">
         <f t="shared" si="1"/>
-        <v>-9.7324360517554401E-2</v>
-      </c>
-      <c r="E5" s="75">
+        <v>-9.1086936740078506E-2</v>
+      </c>
+      <c r="E5" s="73">
         <f t="shared" si="1"/>
-        <v>-9.1894583020425705E-2</v>
+        <v>-9.1114556856590104E-2</v>
       </c>
       <c r="G5" s="18">
         <f>+C6/$B6</f>
@@ -2173,21 +2441,33 @@
         <f>+E6/$B6</f>
         <v>0.13736843489130302</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K5" s="80">
+        <v>2.3825693796604801E-2</v>
+      </c>
+      <c r="L5" s="80">
+        <v>8.7913295104061095E-2</v>
+      </c>
+      <c r="M5" s="80">
+        <v>9.5241393813421102E-2</v>
+      </c>
+      <c r="N5" s="80">
+        <v>7.0074395414781599E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="74">
+      <c r="B6" s="72">
         <v>0.25355954851870199</v>
       </c>
-      <c r="C6" s="74">
+      <c r="C6" s="72">
         <v>0.48810321482980101</v>
       </c>
-      <c r="D6" s="74">
+      <c r="D6" s="72">
         <v>0.76663404311067596</v>
       </c>
-      <c r="E6" s="74">
+      <c r="E6" s="72">
         <v>3.4831078331759503E-2</v>
       </c>
       <c r="G6" s="18">
@@ -2203,110 +2483,158 @@
         <v>0.35047134189088008</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="75">
-        <f>+-G9</f>
-        <v>-3.6007782107965597E-2</v>
-      </c>
-      <c r="C7" s="75">
-        <f t="shared" ref="C7:E7" si="2">+-H9</f>
-        <v>-0.106732211233662</v>
-      </c>
-      <c r="D7" s="75">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="73">
+        <f>+K8</f>
+        <v>-2.3825693796604801E-2</v>
+      </c>
+      <c r="C7" s="73">
+        <f t="shared" ref="C7:E7" si="2">+L8</f>
+        <v>-0.102623074984331</v>
+      </c>
+      <c r="D7" s="73">
         <f t="shared" si="2"/>
-        <v>-9.9568615714996894E-2</v>
-      </c>
-      <c r="E7" s="75">
+        <v>-9.9970167180033806E-2</v>
+      </c>
+      <c r="E7" s="73">
         <f t="shared" si="2"/>
-        <v>-0.124123017797548</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>-0.131180946644253</v>
+      </c>
+      <c r="K7" s="80">
+        <f>-K3</f>
+        <v>-2.3825693796604801E-2</v>
+      </c>
+      <c r="L7" s="80">
+        <f t="shared" ref="L7:N7" si="3">-L3</f>
+        <v>-8.6462761603051996E-2</v>
+      </c>
+      <c r="M7" s="80">
+        <f t="shared" si="3"/>
+        <v>-9.1086936740078506E-2</v>
+      </c>
+      <c r="N7" s="80">
+        <f t="shared" si="3"/>
+        <v>-9.1114556856590104E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="74">
+      <c r="B8" s="72">
         <v>0.25355954851870199</v>
       </c>
-      <c r="C8" s="74">
+      <c r="C8" s="72">
         <v>1.01519994788864</v>
       </c>
-      <c r="D8" s="74">
+      <c r="D8" s="72">
         <v>0.141187788574658</v>
       </c>
-      <c r="E8" s="74">
+      <c r="E8" s="72">
         <v>8.8865355218595204E-2</v>
       </c>
-      <c r="G8" s="77">
-        <v>4.0630067214601502E-2</v>
-      </c>
-      <c r="H8" s="77">
-        <v>8.3571611908693402E-2</v>
-      </c>
-      <c r="I8" s="77">
-        <v>9.7324360517554401E-2</v>
-      </c>
-      <c r="J8" s="77">
-        <v>9.1894583020425705E-2</v>
-      </c>
-      <c r="K8" s="77"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G8" s="80">
+        <v>0.250506013088374</v>
+      </c>
+      <c r="H8" s="80">
+        <v>0.27695568077675098</v>
+      </c>
+      <c r="I8" s="80">
+        <v>0.83798797041589701</v>
+      </c>
+      <c r="J8" s="75">
+        <v>0.26330301045276699</v>
+      </c>
+      <c r="K8" s="80">
+        <f t="shared" ref="K8:N8" si="4">-K4</f>
+        <v>-2.3825693796604801E-2</v>
+      </c>
+      <c r="L8" s="80">
+        <f t="shared" si="4"/>
+        <v>-0.102623074984331</v>
+      </c>
+      <c r="M8" s="80">
+        <f t="shared" si="4"/>
+        <v>-9.9970167180033806E-2</v>
+      </c>
+      <c r="N8" s="80">
+        <f t="shared" si="4"/>
+        <v>-0.131180946644253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19"/>
-      <c r="B9" s="76">
-        <f>-G10</f>
-        <v>-3.4757427098277102E-2</v>
-      </c>
-      <c r="C9" s="76">
-        <f t="shared" ref="C9:E9" si="3">-H10</f>
-        <v>-9.6253137771482297E-2</v>
-      </c>
-      <c r="D9" s="76">
-        <f t="shared" si="3"/>
-        <v>-0.102214538826463</v>
-      </c>
-      <c r="E9" s="76">
-        <f t="shared" si="3"/>
-        <v>-7.0983830304353304E-2</v>
-      </c>
-      <c r="G9" s="77">
-        <v>3.6007782107965597E-2</v>
-      </c>
-      <c r="H9" s="77">
-        <v>0.106732211233662</v>
-      </c>
-      <c r="I9" s="77">
-        <v>9.9568615714996894E-2</v>
-      </c>
-      <c r="J9" s="77">
-        <v>0.124123017797548</v>
-      </c>
-      <c r="K9" s="77"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G10" s="77">
-        <v>3.4757427098277102E-2</v>
-      </c>
-      <c r="H10" s="77">
-        <v>9.6253137771482297E-2</v>
-      </c>
-      <c r="I10" s="77">
-        <v>0.102214538826463</v>
-      </c>
-      <c r="J10" s="77">
-        <v>7.0983830304353304E-2</v>
-      </c>
-      <c r="K10" s="77"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B9" s="74">
+        <f>+K9</f>
+        <v>-2.3825693796604801E-2</v>
+      </c>
+      <c r="C9" s="74">
+        <f t="shared" ref="C9:E9" si="5">+L9</f>
+        <v>-8.7913295104061095E-2</v>
+      </c>
+      <c r="D9" s="74">
+        <f t="shared" si="5"/>
+        <v>-9.5241393813421102E-2</v>
+      </c>
+      <c r="E9" s="74">
+        <f t="shared" si="5"/>
+        <v>-7.0074395414781599E-3</v>
+      </c>
+      <c r="G9" s="80">
+        <v>0.250506013088374</v>
+      </c>
+      <c r="H9" s="80">
+        <v>0.489870693201512</v>
+      </c>
+      <c r="I9" s="80">
+        <v>0.77794346839460005</v>
+      </c>
+      <c r="J9" s="75">
+        <v>2.3903857171145598E-2</v>
+      </c>
+      <c r="K9" s="80">
+        <f t="shared" ref="K9:N9" si="6">-K5</f>
+        <v>-2.3825693796604801E-2</v>
+      </c>
+      <c r="L9" s="80">
+        <f t="shared" si="6"/>
+        <v>-8.7913295104061095E-2</v>
+      </c>
+      <c r="M9" s="80">
+        <f t="shared" si="6"/>
+        <v>-9.5241393813421102E-2</v>
+      </c>
+      <c r="N9" s="80">
+        <f t="shared" si="6"/>
+        <v>-7.0074395414781599E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G10" s="80">
+        <v>0.250506013088374</v>
+      </c>
+      <c r="H10" s="80">
+        <v>1.0339386129405901</v>
+      </c>
+      <c r="I10" s="80">
+        <v>0.127777976759439</v>
+      </c>
+      <c r="J10" s="75">
+        <v>8.5955322866406697E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B11" s="54" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
@@ -2323,20 +2651,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B13" s="54">
         <v>62</v>
       </c>
-      <c r="G13" s="92" t="s">
+      <c r="G13" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-    </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="84"/>
+      <c r="I13" s="84"/>
+      <c r="M13" s="81"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G14" s="8" t="s">
         <v>4</v>
       </c>
@@ -2347,38 +2676,38 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="93" t="s">
+    <row r="15" spans="1:14" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
       <c r="G15" s="18">
-        <f t="shared" ref="G15:I17" si="4">+C18/$B18</f>
+        <f t="shared" ref="G15:I17" si="7">+C18/$B18</f>
         <v>2.2692799840412765</v>
       </c>
       <c r="H15" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.389518623297354</v>
       </c>
       <c r="I15" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.0096069126124061E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G16" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.4104194790539126</v>
       </c>
       <c r="H16" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.1527236641653915</v>
       </c>
       <c r="I16" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.2404717945099751E-2</v>
       </c>
     </row>
@@ -2399,15 +2728,15 @@
         <v>6</v>
       </c>
       <c r="G17" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.952135105688277</v>
       </c>
       <c r="H17" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.4224332808744315</v>
       </c>
       <c r="I17" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.992433008205325E-2</v>
       </c>
     </row>
@@ -2498,11 +2827,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="92" t="s">
+      <c r="G24" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="84"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -2528,23 +2857,23 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="93" t="s">
+      <c r="A26" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="93"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="93"/>
+      <c r="B26" s="98"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="98"/>
       <c r="G26" s="18">
-        <f t="shared" ref="G26:I28" si="5">+C29/$B29</f>
+        <f t="shared" ref="G26:I28" si="8">+C29/$B29</f>
         <v>1.0840988998256753</v>
       </c>
       <c r="H26" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.7002892687797702</v>
       </c>
       <c r="I26" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.85609510095769148</v>
       </c>
       <c r="L26">
@@ -2560,17 +2889,17 @@
         <v>3.5119315719301103E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G27" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.2651573917720484</v>
       </c>
       <c r="H27" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.6005843591077697</v>
       </c>
       <c r="I27" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.16090197814497112</v>
       </c>
       <c r="L27">
@@ -2603,15 +2932,15 @@
         <v>6</v>
       </c>
       <c r="G28" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.1755689228525847</v>
       </c>
       <c r="H28" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.63094595006553655</v>
       </c>
       <c r="I28" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.38561453292854309</v>
       </c>
     </row>
@@ -2667,7 +2996,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>140</v>
       </c>
@@ -2675,7 +3004,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>19</v>
       </c>
@@ -2692,41 +3021,41 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B35" s="1">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="93" t="s">
+    <row r="37" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="93"/>
-      <c r="C37" s="93"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="93"/>
-    </row>
-    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="92" t="s">
+      <c r="B37" s="98"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="98"/>
+    </row>
+    <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G38" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="92"/>
-      <c r="I38" s="92"/>
-    </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H38" s="84"/>
+      <c r="I38" s="84"/>
+    </row>
+    <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
         <v>8</v>
       </c>
@@ -2752,21 +3081,33 @@
       <c r="I39" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K39" s="80">
+        <v>1.8856321828307002E-2</v>
+      </c>
+      <c r="L39" s="80">
+        <v>7.4986834877180303E-2</v>
+      </c>
+      <c r="M39" s="80">
+        <v>0.114521497868232</v>
+      </c>
+      <c r="N39" s="80">
+        <v>0.14262511117377299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="74">
+      <c r="B40" s="72">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C40" s="74">
+      <c r="C40" s="72">
         <v>0.38983157888076198</v>
       </c>
-      <c r="D40" s="74">
+      <c r="D40" s="72">
         <v>0.77387006959986604</v>
       </c>
-      <c r="E40" s="74">
+      <c r="E40" s="72">
         <v>0.132595645940602</v>
       </c>
       <c r="G40" s="18">
@@ -2781,23 +3122,35 @@
         <f>+E40/$B40</f>
         <v>0.44195001212354601</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B41" s="75">
-        <f>-G45</f>
-        <v>-3.27791808747964E-2</v>
-      </c>
-      <c r="C41" s="75">
-        <f t="shared" ref="C41:E41" si="6">-H45</f>
-        <v>-7.5396741976460305E-2</v>
-      </c>
-      <c r="D41" s="75">
-        <f t="shared" si="6"/>
-        <v>-0.115293505002319</v>
-      </c>
-      <c r="E41" s="75">
-        <f t="shared" si="6"/>
-        <v>-0.14196233908585501</v>
+      <c r="K40" s="80">
+        <v>1.8856321828307002E-2</v>
+      </c>
+      <c r="L40" s="80">
+        <v>8.6830087745248793E-2</v>
+      </c>
+      <c r="M40" s="80">
+        <v>8.4460871513142702E-2</v>
+      </c>
+      <c r="N40" s="80">
+        <v>9.4961968222837298E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B41" s="73">
+        <f>-K39</f>
+        <v>-1.8856321828307002E-2</v>
+      </c>
+      <c r="C41" s="73">
+        <f t="shared" ref="C41:E41" si="9">-L39</f>
+        <v>-7.4986834877180303E-2</v>
+      </c>
+      <c r="D41" s="73">
+        <f t="shared" si="9"/>
+        <v>-0.114521497868232</v>
+      </c>
+      <c r="E41" s="73">
+        <f t="shared" si="9"/>
+        <v>-0.14262511117377299</v>
       </c>
       <c r="F41" s="18"/>
       <c r="G41" s="18">
@@ -2812,21 +3165,33 @@
         <f>+E42/$B42</f>
         <v>0.23294604046745127</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K41" s="80">
+        <v>1.8856321828307002E-2</v>
+      </c>
+      <c r="L41" s="80">
+        <v>8.2373258308493402E-2</v>
+      </c>
+      <c r="M41" s="80">
+        <v>8.8718987609085004E-2</v>
+      </c>
+      <c r="N41" s="80">
+        <v>3.5278908100360003E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="74">
+      <c r="B42" s="72">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C42" s="74">
+      <c r="C42" s="72">
         <v>0.536012038389163</v>
       </c>
-      <c r="D42" s="74">
+      <c r="D42" s="72">
         <v>0.65158108175637797</v>
       </c>
-      <c r="E42" s="74">
+      <c r="E42" s="72">
         <v>6.9889421558501405E-2</v>
       </c>
       <c r="G42" s="18">
@@ -2841,115 +3206,125 @@
         <f>+E44/$B44</f>
         <v>0.15281934113026216</v>
       </c>
-      <c r="K42" s="77"/>
-    </row>
-    <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="75">
-        <f>-G46</f>
-        <v>-3.5902339137002803E-2</v>
-      </c>
-      <c r="C43" s="75">
-        <f t="shared" ref="C43:E43" si="7">-H46</f>
-        <v>-8.7285450730600303E-2</v>
-      </c>
-      <c r="D43" s="75">
-        <f t="shared" si="7"/>
-        <v>-8.3582228841739506E-2</v>
-      </c>
-      <c r="E43" s="75">
-        <f t="shared" si="7"/>
-        <v>-9.8175524348070906E-2</v>
-      </c>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="K43" s="77"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K42" s="75"/>
+    </row>
+    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="73">
+        <f>-K40</f>
+        <v>-1.8856321828307002E-2</v>
+      </c>
+      <c r="C43" s="73">
+        <f t="shared" ref="C43:E43" si="10">-L40</f>
+        <v>-8.6830087745248793E-2</v>
+      </c>
+      <c r="D43" s="73">
+        <f t="shared" si="10"/>
+        <v>-8.4460871513142702E-2</v>
+      </c>
+      <c r="E43" s="73">
+        <f t="shared" si="10"/>
+        <v>-9.4961968222837298E-2</v>
+      </c>
+      <c r="F43" s="81"/>
+      <c r="G43" s="82"/>
+      <c r="H43" s="82"/>
+      <c r="I43" s="82"/>
+      <c r="J43" s="81"/>
+      <c r="K43" s="75"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="74">
+      <c r="B44" s="72">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C44" s="74">
+      <c r="C44" s="72">
         <v>0.62828630817505104</v>
       </c>
-      <c r="D44" s="74">
+      <c r="D44" s="72">
         <v>0.55193979369233104</v>
       </c>
-      <c r="E44" s="74">
+      <c r="E44" s="72">
         <v>4.5849482279728501E-2</v>
       </c>
-      <c r="K44" s="77"/>
-    </row>
-    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F44" s="81"/>
+      <c r="G44" s="81"/>
+      <c r="H44" s="81"/>
+      <c r="I44" s="81"/>
+      <c r="J44" s="81"/>
+      <c r="K44" s="75"/>
+    </row>
+    <row r="45" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="19"/>
-      <c r="B45" s="76">
-        <f>-G47</f>
-        <v>-3.5398027084865398E-2</v>
-      </c>
-      <c r="C45" s="76">
-        <f t="shared" ref="C45:E45" si="8">-H47</f>
+      <c r="B45" s="74">
+        <f t="array" ref="B45">-K41:N41</f>
+        <v>-1.8856321828307002E-2</v>
+      </c>
+      <c r="C45" s="74">
+        <f t="shared" ref="C45:E45" si="11">-H47</f>
         <v>-8.8625088080741696E-2</v>
       </c>
-      <c r="D45" s="76">
-        <f t="shared" si="8"/>
+      <c r="D45" s="74">
+        <f t="shared" si="11"/>
         <v>-8.7677991056143698E-2</v>
       </c>
-      <c r="E45" s="76">
-        <f t="shared" si="8"/>
+      <c r="E45" s="74">
+        <f t="shared" si="11"/>
         <v>-7.5233432632621805E-2</v>
       </c>
-      <c r="G45" s="78">
+      <c r="F45" s="81"/>
+      <c r="G45" s="83">
         <v>3.27791808747964E-2</v>
       </c>
-      <c r="H45" s="78">
+      <c r="H45" s="83">
         <v>7.5396741976460305E-2</v>
       </c>
-      <c r="I45" s="78">
+      <c r="I45" s="83">
         <v>0.115293505002319</v>
       </c>
-      <c r="J45" s="77">
+      <c r="J45" s="80">
         <v>0.14196233908585501</v>
       </c>
-      <c r="K45" s="77"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G46" s="77">
+      <c r="K45" s="75"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F46" s="81"/>
+      <c r="G46" s="80">
         <v>3.5902339137002803E-2</v>
       </c>
-      <c r="H46" s="77">
+      <c r="H46" s="80">
         <v>8.7285450730600303E-2</v>
       </c>
-      <c r="I46" s="77">
+      <c r="I46" s="80">
         <v>8.3582228841739506E-2</v>
       </c>
-      <c r="J46" s="77">
+      <c r="J46" s="80">
         <v>9.8175524348070906E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B47" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="G47" s="77">
+      <c r="F47" s="81"/>
+      <c r="G47" s="80">
         <v>3.5398027084865398E-2</v>
       </c>
-      <c r="H47" s="77">
+      <c r="H47" s="80">
         <v>8.8625088080741696E-2</v>
       </c>
-      <c r="I47" s="77">
+      <c r="I47" s="80">
         <v>8.7677991056143698E-2</v>
       </c>
-      <c r="J47" s="77">
+      <c r="J47" s="80">
         <v>7.5233432632621805E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>19</v>
       </c>
@@ -2965,10 +3340,10 @@
       <c r="E48" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="G48" s="77"/>
-      <c r="H48" s="77"/>
-      <c r="I48" s="77"/>
-      <c r="J48" s="77"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
+      <c r="I48" s="75"/>
+      <c r="J48" s="75"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
@@ -2982,20 +3357,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A51" s="93" t="s">
+      <c r="A51" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="93"/>
-      <c r="C51" s="93"/>
-      <c r="D51" s="93"/>
-      <c r="E51" s="93"/>
+      <c r="B51" s="98"/>
+      <c r="C51" s="98"/>
+      <c r="D51" s="98"/>
+      <c r="E51" s="98"/>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="92" t="s">
+      <c r="G52" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="92"/>
-      <c r="I52" s="92"/>
+      <c r="H52" s="84"/>
+      <c r="I52" s="84"/>
     </row>
     <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -3040,15 +3415,15 @@
         <v>0.15027534446115601</v>
       </c>
       <c r="G54" s="18">
-        <f t="shared" ref="G54:G56" si="9">+C54/$B54</f>
+        <f t="shared" ref="G54:G56" si="12">+C54/$B54</f>
         <v>1.373671978812486</v>
       </c>
       <c r="H54" s="18">
-        <f t="shared" ref="H54:H56" si="10">+D54/$B54</f>
+        <f t="shared" ref="H54:H56" si="13">+D54/$B54</f>
         <v>2.882317701442024</v>
       </c>
       <c r="I54" s="18">
-        <f t="shared" ref="I54:I56" si="11">+E54/$B54</f>
+        <f t="shared" ref="I54:I56" si="14">+E54/$B54</f>
         <v>0.54826548178845746</v>
       </c>
     </row>
@@ -3069,15 +3444,15 @@
         <v>7.8971052048355805E-2</v>
       </c>
       <c r="G55" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2.1206583692359722</v>
       </c>
       <c r="H55" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.2750245955063209</v>
       </c>
       <c r="I55" s="18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.28811846716361922</v>
       </c>
     </row>
@@ -3098,15 +3473,15 @@
         <v>0.13010063352593601</v>
       </c>
       <c r="G56" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.8654374748940057</v>
       </c>
       <c r="H56" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.2505536369075858</v>
       </c>
       <c r="I56" s="18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.47465994356458474</v>
       </c>
     </row>
@@ -3319,7 +3694,7 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3338,20 +3713,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="92" t="s">
+      <c r="G4" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -3529,10 +3904,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3543,6 +3918,7 @@
     <col min="5" max="5" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.36328125" customWidth="1"/>
+    <col min="12" max="12" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -3723,16 +4099,16 @@
     <row r="16" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="L16" s="35"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L17" s="35"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
@@ -3748,12 +4124,21 @@
       <c r="E18" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="88"/>
       <c r="L18" s="35"/>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K19" t="s">
+        <v>290</v>
+      </c>
+      <c r="O19" s="79"/>
+      <c r="P19" s="88" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q19" s="88"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="40"/>
       <c r="C20" s="10" t="s">
         <v>63</v>
@@ -3768,11 +4153,22 @@
         <v>129</v>
       </c>
       <c r="I20" s="5">
+        <f>+I23-I21</f>
         <v>86</v>
       </c>
+      <c r="K20" t="s">
+        <v>283</v>
+      </c>
       <c r="L20" s="35"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="O20" s="23"/>
+      <c r="P20" s="78" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q20" s="78" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B21" s="35">
         <v>0.01</v>
       </c>
@@ -3791,8 +4187,20 @@
       <c r="I21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K21" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="O21" s="79" t="s">
+        <v>278</v>
+      </c>
+      <c r="P21">
+        <v>28</v>
+      </c>
+      <c r="Q21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B22" s="35">
         <v>0.05</v>
       </c>
@@ -3800,9 +4208,20 @@
         <v>-2.0304549999999999</v>
       </c>
       <c r="F22" s="28"/>
-      <c r="L22" s="35"/>
-    </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K22" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="O22" s="79" t="s">
+        <v>279</v>
+      </c>
+      <c r="P22">
+        <v>58</v>
+      </c>
+      <c r="Q22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="35">
         <v>0.1</v>
       </c>
@@ -3819,12 +4238,13 @@
         <v>71</v>
       </c>
       <c r="I23" s="19">
-        <f>+SUM(I20:I21)</f>
         <v>93</v>
       </c>
-      <c r="L23" s="35"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K23" s="35" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B24" s="35">
         <v>0.25</v>
       </c>
@@ -3837,14 +4257,18 @@
       <c r="F24" s="28">
         <v>1.168353</v>
       </c>
-      <c r="L24" s="35"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K24" s="35" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="F25" s="28"/>
-      <c r="L25" s="35"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B26" s="35">
         <v>0.5</v>
       </c>
@@ -3857,8 +4281,11 @@
       <c r="F26" s="28">
         <v>1.365048</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="E27" t="s">
         <v>69</v>
@@ -3867,7 +4294,7 @@
         <v>-0.3439432</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="35">
         <v>0.75</v>
       </c>
@@ -3881,7 +4308,7 @@
         <v>13.51919</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B29" s="35">
         <v>0.9</v>
       </c>
@@ -3889,7 +4316,7 @@
         <v>0.87319409999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B30" s="35">
         <v>0.95</v>
       </c>
@@ -3897,7 +4324,7 @@
         <v>1.177781</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="45">
         <v>0.99</v>
       </c>
@@ -3905,39 +4332,41 @@
         <v>5.731446</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="E32" s="35"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E33" s="35"/>
+    </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E34" s="35"/>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E35" s="35"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E36" s="35"/>
-    </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E37" s="35"/>
     </row>
     <row r="39" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E39" s="35"/>
     </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E40" s="35"/>
+    </row>
     <row r="41" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E41" s="35"/>
     </row>
     <row r="42" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E42" s="35"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E43" s="35"/>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E44" s="35"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="H18:I18"/>
+    <mergeCell ref="P19:Q19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3948,8 +4377,8 @@
   </sheetPr>
   <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:Q36"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4324,12 +4753,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4528,8 +4957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F0097E-5ADA-4F9F-8E43-EFEAF7A70026}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4552,14 +4981,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="66" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="76" t="s">
         <v>73</v>
       </c>
       <c r="B4" t="s">
@@ -4570,7 +4999,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="76" t="s">
         <v>72</v>
       </c>
       <c r="B5" t="s">
@@ -4581,7 +5010,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="76" t="s">
         <v>41</v>
       </c>
       <c r="B6" t="s">
@@ -4592,12 +5021,12 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="67" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="76" t="s">
         <v>81</v>
       </c>
       <c r="B8" t="s">
@@ -4608,7 +5037,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="76" t="s">
         <v>47</v>
       </c>
       <c r="B9" t="s">
@@ -4619,7 +5048,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="76" t="s">
         <v>82</v>
       </c>
       <c r="B10" t="s">
@@ -4630,7 +5059,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="76" t="s">
         <v>83</v>
       </c>
       <c r="B11" t="s">
@@ -4641,7 +5070,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="76" t="s">
         <v>50</v>
       </c>
       <c r="B12" t="s">
@@ -4652,7 +5081,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="76" t="s">
         <v>51</v>
       </c>
       <c r="B13" t="s">
@@ -4663,12 +5092,12 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="67" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="76" t="s">
         <v>79</v>
       </c>
       <c r="B15" t="s">
@@ -4679,7 +5108,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="76" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
@@ -4690,7 +5119,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="76" t="s">
         <v>44</v>
       </c>
       <c r="B17" t="s">
@@ -4701,7 +5130,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="76" t="s">
         <v>80</v>
       </c>
       <c r="B18" t="s">
@@ -4712,12 +5141,12 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="67" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="76" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="s">
@@ -4728,7 +5157,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="76" t="s">
         <v>53</v>
       </c>
       <c r="B21" t="s">
@@ -4739,7 +5168,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="76" t="s">
         <v>74</v>
       </c>
       <c r="B22" t="s">
@@ -4750,7 +5179,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="76" t="s">
         <v>75</v>
       </c>
       <c r="B23" t="s">
@@ -4761,7 +5190,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="76" t="s">
         <v>76</v>
       </c>
       <c r="B24" t="s">
@@ -4772,7 +5201,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="76" t="s">
         <v>77</v>
       </c>
       <c r="B25" t="s">
@@ -4783,7 +5212,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="76" t="s">
         <v>58</v>
       </c>
       <c r="B26" t="s">
@@ -4794,7 +5223,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="77" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="41" t="s">
@@ -4818,7 +5247,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="B5:C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -4873,8 +5302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CAF832-E4CD-4D78-919A-B2CAC1381075}">
   <dimension ref="B1:AA34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4893,66 +5322,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="85" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="79" t="s">
+      <c r="H1" s="85" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="N1" s="79" t="s">
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="N1" s="85" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="T1" s="79" t="s">
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="T1" s="85" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="85"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="80" t="s">
+      <c r="H2" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="N2" s="80" t="s">
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="N2" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="T2" s="80" t="s">
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
+      <c r="T2" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="81"/>
-      <c r="X2" s="81"/>
+      <c r="U2" s="87"/>
+      <c r="V2" s="87"/>
+      <c r="W2" s="87"/>
+      <c r="X2" s="87"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -5623,13 +6052,13 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="71" t="s">
+      <c r="I18" s="69" t="s">
         <v>249</v>
       </c>
-      <c r="J18" s="71" t="s">
+      <c r="J18" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="K18" s="71" t="s">
+      <c r="K18" s="69" t="s">
         <v>250</v>
       </c>
       <c r="L18" s="4"/>
@@ -5703,13 +6132,13 @@
       </c>
       <c r="G21" s="58"/>
       <c r="H21" s="58"/>
-      <c r="I21" s="72" t="s">
+      <c r="I21" s="70" t="s">
         <v>245</v>
       </c>
       <c r="J21" s="56">
         <v>93</v>
       </c>
-      <c r="K21" s="72">
+      <c r="K21" s="70">
         <f>+R7/F7</f>
         <v>0.82843257638348444</v>
       </c>
@@ -5897,16 +6326,16 @@
       <c r="B30" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="70">
+      <c r="C30" s="68">
         <v>0.2790882670355333</v>
       </c>
-      <c r="D30" s="70">
+      <c r="D30" s="68">
         <v>0.32358687319242407</v>
       </c>
-      <c r="E30" s="70">
+      <c r="E30" s="68">
         <v>0.41088869394235378</v>
       </c>
-      <c r="F30" s="70">
+      <c r="F30" s="68">
         <v>0.44647090411330181</v>
       </c>
       <c r="G30" s="28"/>
@@ -5971,10 +6400,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DD79C6-8E03-4472-BA01-B1AB9175E2E7}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
   <dimension ref="B2:C65"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5984,10 +6416,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="88" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="82"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -6511,8 +6943,8 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:D42"/>
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6522,13 +6954,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6642,12 +7074,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="84" t="s">
+      <c r="A10" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -6946,12 +7378,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="84" t="s">
+      <c r="A37" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="84"/>
-      <c r="C37" s="84"/>
-      <c r="D37" s="84"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="90"/>
+      <c r="D37" s="90"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -7266,7 +7698,7 @@
   </sheetPr>
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A21" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -7285,13 +7717,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="91" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -7529,13 +7961,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="92"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -7563,13 +7995,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="85" t="s">
+      <c r="A25" s="91" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="85"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -7831,13 +8263,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="86" t="s">
+      <c r="A43" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="86"/>
-      <c r="C43" s="86"/>
-      <c r="D43" s="86"/>
-      <c r="E43" s="86"/>
+      <c r="B43" s="92"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="92"/>
+      <c r="E43" s="92"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -8205,36 +8637,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="87"/>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
-      <c r="Z3" s="87"/>
-      <c r="AA3" s="87"/>
-      <c r="AB3" s="87"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="93"/>
+      <c r="T3" s="93"/>
+      <c r="U3" s="93"/>
+      <c r="V3" s="93"/>
+      <c r="W3" s="93"/>
+      <c r="X3" s="93"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="93"/>
+      <c r="AA3" s="93"/>
+      <c r="AB3" s="93"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -8718,35 +9150,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="91" t="s">
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="88" t="s">
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="89" t="s">
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="89"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="95"/>
+      <c r="T4" s="95"/>
+      <c r="U4" s="95"/>
+      <c r="V4" s="95"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>

<commit_message>
Computed standard errors for sigma
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_7_6.xlsx
+++ b/results/tables/final_tables_7_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F40AC45-6B09-48CF-AED8-84F6C9089331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A102DB5E-187A-466D-B37E-C1C922934E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="7" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="7" activeTab="11" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="294">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -996,6 +996,15 @@
   <si>
     <t>List of occupation</t>
   </si>
+  <si>
+    <t>Estimates</t>
+  </si>
+  <si>
+    <t>t-statistic</t>
+  </si>
+  <si>
+    <t>No sigma is statistically larger than one</t>
+  </si>
 </sst>
 </file>
 
@@ -1007,7 +1016,7 @@
     <numFmt numFmtId="166" formatCode="0.0000_);\(0.0000\)"/>
     <numFmt numFmtId="167" formatCode="0.000_);\(0.000\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1092,6 +1101,14 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1266,7 +1283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1472,6 +1489,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1675,15 +1695,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>531533</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>47812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>232896</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>98781</xdr:rowOff>
+      <xdr:colOff>415179</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>27064</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1706,8 +1726,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="349250" y="6032500"/>
-          <a:ext cx="13440896" cy="9877782"/>
+          <a:off x="531533" y="11554012"/>
+          <a:ext cx="13548846" cy="9224852"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2307,7 +2327,7 @@
   </sheetPr>
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
@@ -3904,10 +3924,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C28" sqref="C18:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3950,7 +3970,9 @@
       <c r="B3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="40"/>
+      <c r="B4" s="10" t="s">
+        <v>291</v>
+      </c>
       <c r="C4" s="10" t="s">
         <v>63</v>
       </c>
@@ -4096,273 +4118,448 @@
       </c>
       <c r="L15" s="35"/>
     </row>
-    <row r="16" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="L16" s="35"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L17" s="35"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B18" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="L18" s="35"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B19" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="L19" s="35"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B20" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="L20" s="35"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B21" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="L21" s="35"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="9"/>
+      <c r="L22" s="35"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B23" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="L23" s="35"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="9"/>
+      <c r="L24" s="35"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B25" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="L25" s="35"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B26" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="L26" s="35"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B27" s="35">
+        <v>0.95</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="L27" s="35"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="45">
+        <v>0.99</v>
+      </c>
+      <c r="C28" s="46"/>
+      <c r="L28" s="35"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="L29" s="35"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L30" s="35"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L31" s="35"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B32" t="s">
         <v>141</v>
       </c>
-      <c r="L17" s="35"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="L32" s="35"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B33" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C33" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D33" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E33" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="88"/>
-      <c r="I18" s="88"/>
-      <c r="L18" s="35"/>
-    </row>
-    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K19" t="s">
+      <c r="H33" s="88"/>
+      <c r="I33" s="88"/>
+      <c r="L33" s="35"/>
+    </row>
+    <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K34" t="s">
         <v>290</v>
       </c>
-      <c r="O19" s="79"/>
-      <c r="P19" s="88" t="s">
+      <c r="O34" s="79"/>
+      <c r="P34" s="88" t="s">
         <v>280</v>
       </c>
-      <c r="Q19" s="88"/>
-    </row>
-    <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="40"/>
-      <c r="C20" s="10" t="s">
+      <c r="Q34" s="88"/>
+    </row>
+    <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="47">
+      <c r="F35" s="47">
         <v>93</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="I20" s="5">
-        <f>+I23-I21</f>
+      <c r="I35" s="5">
+        <f>+I38-I36</f>
         <v>86</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K35" t="s">
         <v>283</v>
       </c>
-      <c r="L20" s="35"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="78" t="s">
+      <c r="L35" s="35"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="Q20" s="78" t="s">
+      <c r="Q35" s="78" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B21" s="35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B36" s="35">
         <v>0.01</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C36" s="9">
         <v>-4.8694680000000004</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E36" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="48">
+      <c r="F36" s="48">
         <v>93</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H36" t="s">
         <v>130</v>
       </c>
-      <c r="I21">
+      <c r="I36">
         <v>7</v>
       </c>
-      <c r="K21" s="35" t="s">
+      <c r="K36" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="O21" s="79" t="s">
+      <c r="O36" s="79" t="s">
         <v>278</v>
       </c>
-      <c r="P21">
+      <c r="P36">
         <v>28</v>
       </c>
-      <c r="Q21">
+      <c r="Q36">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B22" s="35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B37" s="35">
         <v>0.05</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C37" s="9">
         <v>-2.0304549999999999</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="K22" s="35" t="s">
+      <c r="F37" s="28"/>
+      <c r="K37" s="35" t="s">
         <v>285</v>
       </c>
-      <c r="O22" s="79" t="s">
+      <c r="O37" s="79" t="s">
         <v>279</v>
       </c>
-      <c r="P22">
+      <c r="P37">
         <v>58</v>
       </c>
-      <c r="Q22">
+      <c r="Q37">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="35">
+    <row r="38" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="35">
         <v>0.1</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C38" s="9">
         <v>-0.63951970000000002</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E38" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F38" s="28">
         <v>-1.32762E-2</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H38" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I38" s="19">
         <v>93</v>
       </c>
-      <c r="K23" s="35" t="s">
+      <c r="K38" s="35" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B24" s="35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B39" s="35">
         <v>0.25</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C39" s="9">
         <v>-0.1918347</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E39" t="s">
         <v>67</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F39" s="28">
         <v>1.168353</v>
       </c>
-      <c r="K24" s="35" t="s">
+      <c r="K39" s="35" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="C25" s="9"/>
-      <c r="F25" s="28"/>
-      <c r="K25" t="s">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="C40" s="9"/>
+      <c r="F40" s="28"/>
+      <c r="H40" s="99" t="s">
+        <v>293</v>
+      </c>
+      <c r="I40" s="99"/>
+      <c r="K40" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B26" s="35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B41" s="35">
         <v>0.5</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C41" s="9">
         <v>1.5392599999999999E-2</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E41" t="s">
         <v>68</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F41" s="28">
         <v>1.365048</v>
       </c>
-      <c r="K26" t="s">
+      <c r="H41" s="99"/>
+      <c r="I41" s="99"/>
+      <c r="K41" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="C27" s="9"/>
-      <c r="E27" t="s">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="C42" s="9"/>
+      <c r="E42" t="s">
         <v>69</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F42" s="28">
         <v>-0.3439432</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="35">
+      <c r="H42" s="99"/>
+      <c r="I42" s="99"/>
+    </row>
+    <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="35">
         <v>0.75</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C43" s="9">
         <v>0.36161979999999999</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E43" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="49">
+      <c r="F43" s="49">
         <v>13.51919</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B29" s="35">
+      <c r="H43" s="99"/>
+      <c r="I43" s="99"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B44" s="35">
         <v>0.9</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C44" s="9">
         <v>0.87319409999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B30" s="35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B45" s="35">
         <v>0.95</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C45" s="9">
         <v>1.177781</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="45">
+    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="45">
         <v>0.99</v>
       </c>
-      <c r="C31" s="46">
+      <c r="C46" s="46">
         <v>5.731446</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="E32" s="35"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E33" s="35"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E34" s="35"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E35" s="35"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E37" s="35"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E39" s="35"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E40" s="35"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E41" s="35"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E42" s="35"/>
-    </row>
+    <row r="47" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="E47" s="35"/>
+    </row>
+    <row r="48" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E48" s="35"/>
+    </row>
+    <row r="49" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="35"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B50" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="C50" s="9">
+        <v>-0.85092900000000005</v>
+      </c>
+      <c r="E50" s="35"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="C51" s="9">
+        <v>-0.39615220000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B52" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="C52" s="9">
+        <v>-0.20169000000000001</v>
+      </c>
+      <c r="E52" s="35"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B53" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="C53" s="9">
+        <v>-6.5401100000000004E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C54" s="9"/>
+      <c r="E54" s="35"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B55" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="C55" s="9">
+        <v>2.0936300000000001E-2</v>
+      </c>
+      <c r="E55" s="35"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C56" s="9"/>
+      <c r="E56" s="35"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B57" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="C57" s="9">
+        <v>0.17986369999999999</v>
+      </c>
+      <c r="E57" s="35"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B58" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="C58" s="9">
+        <v>0.55942829999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B59" s="35">
+        <v>0.95</v>
+      </c>
+      <c r="C59" s="9">
+        <v>0.82273249999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="45">
+        <v>0.99</v>
+      </c>
+      <c r="C60" s="46">
+        <v>1.6229610000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="P19:Q19"/>
+  <mergeCells count="3">
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="H40:I43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>